<commit_message>
Updated original data sheet.
A few rows were appended to the wrong part of the file.
</commit_message>
<xml_diff>
--- a/Voight et al original data.xlsx
+++ b/Voight et al original data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvoight\Dropbox (The Field Museum)\My Files 2017\MS\isotope\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11295"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11295" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="chimney size fract" sheetId="3" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="wood" sheetId="4" r:id="rId3"/>
     <sheet name="Summary" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="181">
   <si>
     <t>Name</t>
   </si>
@@ -189,9 +184,6 @@
   </si>
   <si>
     <t>X wash 3.raw</t>
-  </si>
-  <si>
-    <t>X wash 5 shell.raw</t>
   </si>
   <si>
     <t>large dorsalis investigate isotope values of cecum contents</t>
@@ -1225,7 +1217,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1235,8 +1227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1290,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1335,7 +1327,7 @@
         <v>1.1209450305346726</v>
       </c>
       <c r="I4" s="8">
-        <f>E4/H4</f>
+        <f t="shared" ref="I4:I9" si="0">E4/H4</f>
         <v>53.640293595243321</v>
       </c>
     </row>
@@ -1365,7 +1357,7 @@
         <v>0.99690672325165997</v>
       </c>
       <c r="I5" s="8">
-        <f>E5/H5</f>
+        <f t="shared" si="0"/>
         <v>51.322351638317819</v>
       </c>
     </row>
@@ -1395,7 +1387,7 @@
         <v>0.30359230705702378</v>
       </c>
       <c r="I6" s="8">
-        <f>E6/H6</f>
+        <f t="shared" si="0"/>
         <v>74.200056767781149</v>
       </c>
     </row>
@@ -1425,7 +1417,7 @@
         <v>0.47324924541226338</v>
       </c>
       <c r="I7" s="8">
-        <f>E7/H7</f>
+        <f t="shared" si="0"/>
         <v>81.973505960843283</v>
       </c>
     </row>
@@ -1455,7 +1447,7 @@
         <v>1.4729561881363313</v>
       </c>
       <c r="I8" s="8">
-        <f>E8/H8</f>
+        <f t="shared" si="0"/>
         <v>18.909292264743797</v>
       </c>
     </row>
@@ -1485,7 +1477,7 @@
         <v>3.0441232627123895</v>
       </c>
       <c r="I9" s="8">
-        <f>E9/H9</f>
+        <f t="shared" si="0"/>
         <v>43.636752622822428</v>
       </c>
     </row>
@@ -1572,7 +1564,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1586,7 +1578,7 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="8">
         <v>2.5602024999999999</v>
@@ -1614,7 +1606,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="8">
         <v>1.2257828749999999</v>
@@ -1642,7 +1634,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8">
         <v>0.59160000000000001</v>
@@ -1670,7 +1662,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="8">
         <v>4.1791697499999998</v>
@@ -1698,7 +1690,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="8">
         <v>3.9981452499999999</v>
@@ -1730,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,7 +1983,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -2060,10 +2052,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="C15" s="8">
         <v>3.2442394999999999</v>
@@ -2090,10 +2082,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>76</v>
       </c>
       <c r="C16" s="8">
         <v>7.8962994999999996</v>
@@ -2118,12 +2110,12 @@
         <v>351.5543769201347</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>81</v>
       </c>
       <c r="C18" s="8">
         <v>5.5022289999999998</v>
@@ -2148,9 +2140,9 @@
         <v>263.36290106236521</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -2161,6 +2153,70 @@
       <c r="H19" s="30"/>
       <c r="I19" s="8"/>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="8">
+        <v>4.4432914999999999</v>
+      </c>
+      <c r="D20" s="8">
+        <v>-25.864419699042745</v>
+      </c>
+      <c r="E20" s="30">
+        <v>43.913058751302607</v>
+      </c>
+      <c r="F20" s="11">
+        <v>7.4600265624999995E-2</v>
+      </c>
+      <c r="G20" s="11">
+        <v>-0.32380655991678176</v>
+      </c>
+      <c r="H20" s="30">
+        <v>0.43792060860380222</v>
+      </c>
+      <c r="I20" s="8">
+        <f>E20/H20</f>
+        <v>100.27630097452631</v>
+      </c>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="8">
+        <v>11.021521</v>
+      </c>
+      <c r="D21" s="8">
+        <v>-25.998018902671401</v>
+      </c>
+      <c r="E21" s="30">
+        <v>109.2401890748493</v>
+      </c>
+      <c r="F21" s="11">
+        <v>0.1086961171875</v>
+      </c>
+      <c r="G21" s="11">
+        <v>0.72893756206437932</v>
+      </c>
+      <c r="H21" s="30">
+        <v>0.60581940897525566</v>
+      </c>
+      <c r="I21" s="8">
+        <f>E21/H21</f>
+        <v>180.31807409344844</v>
+      </c>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2168,10 +2224,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S230"/>
+  <dimension ref="A1:S227"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,7 +2563,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -2788,7 +2844,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2803,7 +2859,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2908,7 +2964,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2983,7 +3039,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3058,10 +3114,10 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>78</v>
       </c>
       <c r="C35" s="8">
         <v>1.36474725</v>
@@ -3090,10 +3146,10 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C36" s="8">
         <v>1.94544275</v>
@@ -3135,7 +3191,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3306,551 +3362,527 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="8">
-        <v>0.73169899999999999</v>
-      </c>
-      <c r="D43" s="8">
-        <v>-21.581690770000002</v>
-      </c>
-      <c r="E43" s="8">
-        <v>9.1917979770000002</v>
-      </c>
-      <c r="F43" s="8">
-        <v>0.28317487499999999</v>
-      </c>
-      <c r="G43" s="8">
-        <v>5.4996754699999997</v>
-      </c>
-      <c r="H43" s="8">
-        <v>2.1895950759999998</v>
-      </c>
-      <c r="I43" s="8">
-        <v>4.1980000000000004</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="A44" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="8">
+        <v>3.2949985000000002</v>
+      </c>
+      <c r="D44" s="8">
+        <v>-26.082252991078715</v>
+      </c>
+      <c r="E44" s="8">
+        <v>31.853204608183603</v>
+      </c>
+      <c r="F44" s="8">
+        <v>1.496072375</v>
+      </c>
+      <c r="G44" s="8">
+        <v>6.1327562941884413</v>
+      </c>
+      <c r="H44" s="8">
+        <v>8.501340250751154</v>
+      </c>
+      <c r="I44" s="8">
+        <f>E44/H44</f>
+        <v>3.7468450466229895</v>
+      </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>62</v>
       </c>
       <c r="C45" s="8">
-        <v>3.2949985000000002</v>
+        <v>7.9100064999999997</v>
       </c>
       <c r="D45" s="8">
-        <v>-26.082252991078715</v>
+        <v>-26.611187188018175</v>
       </c>
       <c r="E45" s="8">
-        <v>31.853204608183603</v>
+        <v>77.532015264072882</v>
       </c>
       <c r="F45" s="8">
-        <v>1.496072375</v>
+        <v>3.1982932499999999</v>
       </c>
       <c r="G45" s="8">
-        <v>6.1327562941884413</v>
+        <v>1.4992035891583113</v>
       </c>
       <c r="H45" s="8">
-        <v>8.501340250751154</v>
+        <v>18.910235622862128</v>
       </c>
       <c r="I45" s="8">
         <f>E45/H45</f>
-        <v>3.7468450466229895</v>
+        <v>4.1000026023122684</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C46" s="8">
-        <v>7.9100064999999997</v>
+        <v>6.3656905000000004</v>
       </c>
       <c r="D46" s="8">
-        <v>-26.611187188018175</v>
+        <v>-25.04924994052741</v>
       </c>
       <c r="E46" s="8">
-        <v>77.532015264072882</v>
+        <v>61.552750575916647</v>
       </c>
       <c r="F46" s="8">
-        <v>3.1982932499999999</v>
+        <v>2.6379777500000001</v>
       </c>
       <c r="G46" s="8">
-        <v>1.4992035891583113</v>
+        <v>1.3934855298177158</v>
       </c>
       <c r="H46" s="8">
-        <v>18.910235622862128</v>
+        <v>15.774954682689769</v>
       </c>
       <c r="I46" s="8">
         <f>E46/H46</f>
-        <v>4.1000026023122684</v>
+        <v>3.9019288368200473</v>
       </c>
       <c r="J46" s="8"/>
       <c r="K46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C47" s="8">
-        <v>6.3656905000000004</v>
-      </c>
-      <c r="D47" s="8">
-        <v>-25.04924994052741</v>
-      </c>
-      <c r="E47" s="8">
-        <v>61.552750575916647</v>
-      </c>
-      <c r="F47" s="8">
-        <v>2.6379777500000001</v>
-      </c>
-      <c r="G47" s="8">
-        <v>1.3934855298177158</v>
-      </c>
-      <c r="H47" s="8">
-        <v>15.774954682689769</v>
-      </c>
-      <c r="I47" s="8">
-        <f>E47/H47</f>
-        <v>3.9019288368200473</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="8">
+        <v>1.5157242500000001</v>
+      </c>
+      <c r="D48" s="8">
+        <v>-22.402100564240747</v>
+      </c>
+      <c r="E48" s="8">
+        <v>14.938791023148589</v>
+      </c>
+      <c r="F48" s="8">
+        <v>0.45145553124999999</v>
+      </c>
+      <c r="G48" s="8">
+        <v>0.77586006528551354</v>
+      </c>
+      <c r="H48" s="8">
+        <v>2.8531195546213759</v>
+      </c>
+      <c r="I48" s="8">
+        <f>E48/H48</f>
+        <v>5.235949891742635</v>
+      </c>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C49" s="8">
-        <v>1.5157242500000001</v>
-      </c>
-      <c r="D49" s="8">
-        <v>-22.402100564240747</v>
-      </c>
-      <c r="E49" s="8">
-        <v>14.938791023148589</v>
-      </c>
-      <c r="F49" s="8">
-        <v>0.45145553124999999</v>
-      </c>
-      <c r="G49" s="8">
-        <v>0.77586006528551354</v>
-      </c>
-      <c r="H49" s="8">
-        <v>2.8531195546213759</v>
-      </c>
-      <c r="I49" s="8">
-        <f>E49/H49</f>
-        <v>5.235949891742635</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
       <c r="J49" s="8"/>
       <c r="K49" s="8"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="8">
+        <v>3.7236319999999998</v>
+      </c>
+      <c r="D50" s="8">
+        <v>-25.25042352806884</v>
+      </c>
+      <c r="E50" s="8">
+        <v>36.224442427222023</v>
+      </c>
+      <c r="F50" s="8">
+        <v>1.422802125</v>
+      </c>
+      <c r="G50" s="8">
+        <v>3.2208339204787788</v>
+      </c>
+      <c r="H50" s="8">
+        <v>8.0561017062061424</v>
+      </c>
+      <c r="I50" s="8">
+        <f>E50/H50</f>
+        <v>4.4965224805088999</v>
+      </c>
       <c r="J50" s="8"/>
       <c r="K50" s="8"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C51" s="8">
-        <v>3.7236319999999998</v>
+        <v>5.0450549999999996</v>
       </c>
       <c r="D51" s="8">
-        <v>-25.25042352806884</v>
+        <v>-24.430691971954726</v>
       </c>
       <c r="E51" s="8">
-        <v>36.224442427222023</v>
+        <v>47.582230674400989</v>
       </c>
       <c r="F51" s="8">
-        <v>1.422802125</v>
+        <v>1.817097</v>
       </c>
       <c r="G51" s="8">
-        <v>3.2208339204787788</v>
+        <v>4.6760724234072644</v>
       </c>
       <c r="H51" s="8">
-        <v>8.0561017062061424</v>
+        <v>10.843067741812201</v>
       </c>
       <c r="I51" s="8">
         <f>E51/H51</f>
-        <v>4.4965224805088999</v>
+        <v>4.3882627875613158</v>
       </c>
       <c r="J51" s="8"/>
       <c r="K51" s="8"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C52" s="8">
-        <v>5.0450549999999996</v>
+        <v>4.1148022500000003</v>
       </c>
       <c r="D52" s="8">
-        <v>-24.430691971954726</v>
-      </c>
-      <c r="E52" s="8">
-        <v>47.582230674400989</v>
-      </c>
-      <c r="F52" s="8">
-        <v>1.817097</v>
-      </c>
-      <c r="G52" s="8">
-        <v>4.6760724234072644</v>
-      </c>
-      <c r="H52" s="8">
-        <v>10.843067741812201</v>
+        <v>-23.839375178648741</v>
+      </c>
+      <c r="E52" s="30">
+        <v>39.169811480802061</v>
+      </c>
+      <c r="F52" s="30">
+        <v>1.450735125</v>
+      </c>
+      <c r="G52" s="30">
+        <v>5.0365902656969128</v>
+      </c>
+      <c r="H52" s="30">
+        <v>8.8957932313055963</v>
       </c>
       <c r="I52" s="8">
         <f>E52/H52</f>
-        <v>4.3882627875613158</v>
+        <v>4.4031836692154407</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C53" s="8">
-        <v>4.1148022500000003</v>
+        <v>2.128876</v>
       </c>
       <c r="D53" s="8">
-        <v>-23.839375178648741</v>
+        <v>-24.438291394616606</v>
       </c>
       <c r="E53" s="30">
-        <v>39.169811480802061</v>
+        <v>20.151186481423881</v>
       </c>
       <c r="F53" s="30">
-        <v>1.450735125</v>
+        <v>0.81578625000000005</v>
       </c>
       <c r="G53" s="30">
-        <v>5.0365902656969128</v>
+        <v>4.6615302846864726</v>
       </c>
       <c r="H53" s="30">
-        <v>8.8957932313055963</v>
+        <v>5.2182964669452225</v>
       </c>
       <c r="I53" s="8">
         <f>E53/H53</f>
-        <v>4.4031836692154407</v>
+        <v>3.8616407881517576</v>
       </c>
       <c r="J53" s="8"/>
       <c r="K53" s="8"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="8">
-        <v>2.128876</v>
-      </c>
-      <c r="D54" s="8">
-        <v>-24.438291394616606</v>
-      </c>
-      <c r="E54" s="30">
-        <v>20.151186481423881</v>
-      </c>
-      <c r="F54" s="30">
-        <v>0.81578625000000005</v>
-      </c>
-      <c r="G54" s="30">
-        <v>4.6615302846864726</v>
-      </c>
-      <c r="H54" s="30">
-        <v>5.2182964669452225</v>
-      </c>
-      <c r="I54" s="8">
-        <f>E54/H54</f>
-        <v>3.8616407881517576</v>
-      </c>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="8">
-        <v>4.4432914999999999</v>
-      </c>
-      <c r="D55" s="8">
-        <v>-25.864419699042745</v>
-      </c>
-      <c r="E55" s="30">
-        <v>43.913058751302607</v>
-      </c>
-      <c r="F55" s="11">
-        <v>7.4600265624999995E-2</v>
-      </c>
-      <c r="G55" s="11">
-        <v>-0.32380655991678176</v>
-      </c>
-      <c r="H55" s="30">
-        <v>0.43792060860380222</v>
-      </c>
-      <c r="I55" s="8">
-        <f>E55/H55</f>
-        <v>100.27630097452631</v>
+        <v>171</v>
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="C56" s="8">
-        <v>11.021521</v>
+        <v>2.5094129999999999</v>
       </c>
       <c r="D56" s="8">
-        <v>-25.998018902671401</v>
-      </c>
-      <c r="E56" s="30">
-        <v>109.2401890748493</v>
-      </c>
-      <c r="F56" s="11">
-        <v>0.1086961171875</v>
-      </c>
-      <c r="G56" s="11">
-        <v>0.72893756206437932</v>
-      </c>
-      <c r="H56" s="30">
-        <v>0.60581940897525566</v>
+        <v>-25.47191136874477</v>
+      </c>
+      <c r="E56" s="8">
+        <v>24.318698879101461</v>
+      </c>
+      <c r="F56" s="8">
+        <v>0.72221868749999996</v>
+      </c>
+      <c r="G56" s="8">
+        <v>3.5250209887373423</v>
+      </c>
+      <c r="H56" s="8">
+        <v>4.2436854104651323</v>
       </c>
       <c r="I56" s="8">
         <f>E56/H56</f>
-        <v>180.31807409344844</v>
+        <v>5.7305611813567472</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C57" s="8">
+        <v>4.0557962500000002</v>
+      </c>
+      <c r="D57" s="8">
+        <v>-25.215621714515635</v>
+      </c>
+      <c r="E57" s="8">
+        <v>38.454702065186446</v>
+      </c>
+      <c r="F57" s="8">
+        <v>1.0808355000000001</v>
+      </c>
+      <c r="G57" s="8">
+        <v>3.4654912710679082</v>
+      </c>
+      <c r="H57" s="8">
+        <v>6.6546680046767257</v>
+      </c>
+      <c r="I57" s="8">
+        <v>5.7786</v>
+      </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>172</v>
+        <v>164</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="8">
+        <v>2.45496925</v>
+      </c>
+      <c r="D58" s="8">
+        <v>-25.250325091228593</v>
+      </c>
+      <c r="E58" s="8">
+        <v>23.23759187717296</v>
+      </c>
+      <c r="F58" s="8">
+        <v>0.66027906250000001</v>
+      </c>
+      <c r="G58" s="8">
+        <v>4.051680187851268</v>
+      </c>
+      <c r="H58" s="8">
+        <v>4.2822089978606641</v>
+      </c>
+      <c r="I58" s="8">
+        <v>5.4264999999999999</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C59" s="8">
-        <v>2.5094129999999999</v>
+        <v>3.6038725</v>
       </c>
       <c r="D59" s="8">
-        <v>-25.47191136874477</v>
+        <v>-25.120543087233479</v>
       </c>
       <c r="E59" s="8">
-        <v>24.318698879101461</v>
+        <v>34.232692726387427</v>
       </c>
       <c r="F59" s="8">
-        <v>0.72221868749999996</v>
+        <v>0.94040056250000004</v>
       </c>
       <c r="G59" s="8">
-        <v>3.5250209887373423</v>
+        <v>3.8502896792648009</v>
       </c>
       <c r="H59" s="8">
-        <v>4.2436854104651323</v>
+        <v>5.8689597934100854</v>
       </c>
       <c r="I59" s="8">
-        <f>E59/H59</f>
-        <v>5.7305611813567472</v>
+        <v>5.8327999999999998</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C60" s="8">
-        <v>4.0557962500000002</v>
-      </c>
-      <c r="D60" s="8">
-        <v>-25.215621714515635</v>
-      </c>
-      <c r="E60" s="8">
-        <v>38.454702065186446</v>
-      </c>
-      <c r="F60" s="8">
-        <v>1.0808355000000001</v>
-      </c>
-      <c r="G60" s="8">
-        <v>3.4654912710679082</v>
-      </c>
-      <c r="H60" s="8">
-        <v>6.6546680046767257</v>
-      </c>
-      <c r="I60" s="8">
-        <v>5.7786</v>
-      </c>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C61" s="8">
-        <v>2.45496925</v>
-      </c>
-      <c r="D61" s="8">
-        <v>-25.250325091228593</v>
-      </c>
-      <c r="E61" s="8">
-        <v>23.23759187717296</v>
-      </c>
-      <c r="F61" s="8">
-        <v>0.66027906250000001</v>
-      </c>
-      <c r="G61" s="8">
-        <v>4.051680187851268</v>
-      </c>
-      <c r="H61" s="8">
-        <v>4.2822089978606641</v>
-      </c>
-      <c r="I61" s="8">
-        <v>5.4264999999999999</v>
-      </c>
+      <c r="A61" s="28" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>164</v>
+        <v>88</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C62" s="8">
-        <v>3.6038725</v>
+        <v>1.9666946249999999</v>
       </c>
       <c r="D62" s="8">
-        <v>-25.120543087233479</v>
+        <v>-23.094487363205179</v>
       </c>
       <c r="E62" s="8">
-        <v>34.232692726387427</v>
+        <v>19.032929356816773</v>
       </c>
       <c r="F62" s="8">
-        <v>0.94040056250000004</v>
+        <v>0.76995000000000002</v>
       </c>
       <c r="G62" s="8">
-        <v>3.8502896792648009</v>
+        <v>1.0641368039767234</v>
       </c>
       <c r="H62" s="8">
-        <v>5.8689597934100854</v>
+        <v>4.5497919678386678</v>
       </c>
       <c r="I62" s="8">
-        <v>5.8327999999999998</v>
+        <f>E62/H62</f>
+        <v>4.1832526610789573</v>
       </c>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C63" s="8">
+        <v>5.0683259999999999</v>
+      </c>
+      <c r="D63" s="8">
+        <v>-23.156006906874545</v>
+      </c>
+      <c r="E63" s="8">
+        <v>49.376705767290389</v>
+      </c>
+      <c r="F63" s="8">
+        <v>2.200828</v>
+      </c>
+      <c r="G63" s="8">
+        <v>1.4616070592425006</v>
+      </c>
+      <c r="H63" s="8">
+        <v>12.332625804389194</v>
+      </c>
+      <c r="I63" s="8">
+        <f>E63/H63</f>
+        <v>4.0037463675997671</v>
+      </c>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="28" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -3865,668 +3897,666 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C65" s="8">
-        <v>1.9666946249999999</v>
+        <v>1.8585257500000001</v>
       </c>
       <c r="D65" s="8">
-        <v>-23.094487363205179</v>
+        <v>-24.286500471833353</v>
       </c>
       <c r="E65" s="8">
-        <v>19.032929356816773</v>
+        <v>22.038718961628859</v>
       </c>
       <c r="F65" s="8">
-        <v>0.76995000000000002</v>
+        <v>0.78421200000000002</v>
       </c>
       <c r="G65" s="8">
-        <v>1.0641368039767234</v>
+        <v>2.0261371570758699</v>
       </c>
       <c r="H65" s="8">
-        <v>4.5497919678386678</v>
+        <v>5.7523093976407553</v>
       </c>
       <c r="I65" s="8">
-        <f>E65/H65</f>
-        <v>4.1832526610789573</v>
+        <v>3.83</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C66" s="8">
-        <v>5.0683259999999999</v>
+        <v>6.684094</v>
       </c>
       <c r="D66" s="8">
-        <v>-23.156006906874545</v>
+        <v>-23.835274678547957</v>
       </c>
       <c r="E66" s="8">
-        <v>49.376705767290389</v>
+        <v>79.765415197696683</v>
       </c>
       <c r="F66" s="8">
-        <v>2.200828</v>
+        <v>2.9344342499999998</v>
       </c>
       <c r="G66" s="8">
-        <v>1.4616070592425006</v>
+        <v>2.083019631112216</v>
       </c>
       <c r="H66" s="8">
-        <v>12.332625804389194</v>
+        <v>20.088894801554094</v>
       </c>
       <c r="I66" s="8">
-        <f>E66/H66</f>
-        <v>4.0037463675997671</v>
+        <v>3.97</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
+      <c r="A67" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="8">
+        <v>3.6916704999999999</v>
+      </c>
+      <c r="D67" s="8">
+        <v>-24.240474740321815</v>
+      </c>
+      <c r="E67" s="8">
+        <v>43.746076299998037</v>
+      </c>
+      <c r="F67" s="8">
+        <v>1.4606551249999999</v>
+      </c>
+      <c r="G67" s="8">
+        <v>0.86986717722235096</v>
+      </c>
+      <c r="H67" s="8">
+        <v>10.369736301493674</v>
+      </c>
+      <c r="I67" s="8">
+        <v>4.22</v>
+      </c>
       <c r="J67" s="8"/>
       <c r="K67" s="8"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="C68" s="8">
-        <v>1.8585257500000001</v>
-      </c>
-      <c r="D68" s="8">
-        <v>-24.286500471833353</v>
-      </c>
-      <c r="E68" s="8">
-        <v>22.038718961628859</v>
-      </c>
-      <c r="F68" s="8">
-        <v>0.78421200000000002</v>
-      </c>
-      <c r="G68" s="8">
-        <v>2.0261371570758699</v>
-      </c>
-      <c r="H68" s="8">
-        <v>5.7523093976407553</v>
-      </c>
-      <c r="I68" s="8">
-        <v>3.83</v>
-      </c>
+      <c r="A68" s="11"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="8">
-        <v>6.684094</v>
-      </c>
-      <c r="D69" s="8">
-        <v>-23.835274678547957</v>
-      </c>
-      <c r="E69" s="8">
-        <v>79.765415197696683</v>
-      </c>
-      <c r="F69" s="8">
-        <v>2.9344342499999998</v>
-      </c>
-      <c r="G69" s="8">
-        <v>2.083019631112216</v>
-      </c>
-      <c r="H69" s="8">
-        <v>20.088894801554094</v>
-      </c>
-      <c r="I69" s="8">
-        <v>3.97</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E69" s="8"/>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>92</v>
+      <c r="A70" s="28" t="s">
+        <v>85</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C70" s="8">
-        <v>3.6916704999999999</v>
+        <v>4.3087499999999999</v>
       </c>
       <c r="D70" s="8">
-        <v>-24.240474740321815</v>
+        <v>-22.841603134997509</v>
       </c>
       <c r="E70" s="8">
-        <v>43.746076299998037</v>
+        <v>42.009365970805867</v>
       </c>
       <c r="F70" s="8">
-        <v>1.4606551249999999</v>
+        <v>1.7290325</v>
       </c>
       <c r="G70" s="8">
-        <v>0.86986717722235096</v>
+        <v>0.23577193624782825</v>
       </c>
       <c r="H70" s="8">
-        <v>10.369736301493674</v>
+        <v>9.7065380809605326</v>
       </c>
       <c r="I70" s="8">
-        <v>4.22</v>
+        <f>E70/H70</f>
+        <v>4.3279453107187251</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
+      <c r="A71" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="8">
+        <v>2.3880970000000001</v>
+      </c>
+      <c r="D71" s="8">
+        <v>-23.089139430027142</v>
+      </c>
+      <c r="E71" s="8">
+        <v>22.95719382001516</v>
+      </c>
+      <c r="F71" s="8">
+        <v>0.97920750000000001</v>
+      </c>
+      <c r="G71" s="8">
+        <v>0.36457644582799265</v>
+      </c>
+      <c r="H71" s="8">
+        <v>5.6530562254791619</v>
+      </c>
+      <c r="I71" s="8">
+        <f>E71/H71</f>
+        <v>4.0610234365870426</v>
+      </c>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="8" t="s">
-        <v>121</v>
-      </c>
+      <c r="D72" s="8"/>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
-      <c r="G72" s="8" t="s">
-        <v>121</v>
-      </c>
+      <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
-        <v>86</v>
+      <c r="A73" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C73" s="8">
-        <v>4.3087499999999999</v>
-      </c>
-      <c r="D73" s="8">
-        <v>-22.841603134997509</v>
+        <v>1.5596851249999999</v>
+      </c>
+      <c r="D73" s="11">
+        <v>-22.465484879424601</v>
       </c>
       <c r="E73" s="8">
-        <v>42.009365970805867</v>
+        <v>18.829710357548414</v>
       </c>
       <c r="F73" s="8">
-        <v>1.7290325</v>
+        <v>0.62700849999999997</v>
       </c>
       <c r="G73" s="8">
-        <v>0.23577193624782825</v>
+        <v>-0.33165162163020123</v>
       </c>
       <c r="H73" s="8">
-        <v>9.7065380809605326</v>
+        <v>4.933828923826284</v>
       </c>
       <c r="I73" s="8">
-        <f>E73/H73</f>
-        <v>4.3279453107187251</v>
+        <v>3.8170000000000002</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" s="28" t="s">
-        <v>86</v>
+      <c r="A74" s="11" t="s">
+        <v>95</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="C74" s="8">
-        <v>2.3880970000000001</v>
-      </c>
-      <c r="D74" s="8">
-        <v>-23.089139430027142</v>
+        <v>2.386304</v>
+      </c>
+      <c r="D74" s="11">
+        <v>-25.298547291521309</v>
       </c>
       <c r="E74" s="8">
-        <v>22.95719382001516</v>
+        <v>28.947319595966892</v>
       </c>
       <c r="F74" s="8">
-        <v>0.97920750000000001</v>
+        <v>0.96525075000000005</v>
       </c>
       <c r="G74" s="8">
-        <v>0.36457644582799265</v>
+        <v>-0.27194060419857169</v>
       </c>
       <c r="H74" s="8">
-        <v>5.6530562254791619</v>
+        <v>7.413621955214146</v>
       </c>
       <c r="I74" s="8">
-        <f>E74/H74</f>
-        <v>4.0610234365870426</v>
+        <v>3.9039999999999999</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
+        <v>95</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C75" s="8">
+        <v>7.6152749999999996</v>
+      </c>
+      <c r="D75" s="11">
+        <v>-25.732896740956409</v>
+      </c>
+      <c r="E75" s="8">
+        <v>90.984209695175196</v>
+      </c>
+      <c r="F75" s="8">
+        <v>3.50915775</v>
+      </c>
+      <c r="G75" s="8">
+        <v>-1.1615637497241138</v>
+      </c>
+      <c r="H75" s="8">
+        <v>24.702444077116027</v>
+      </c>
+      <c r="I75" s="8">
+        <v>3.6829999999999998</v>
+      </c>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C76" s="8">
-        <v>1.5596851249999999</v>
+        <v>4.1858392499999999</v>
       </c>
       <c r="D76" s="11">
-        <v>-22.465484879424601</v>
+        <v>-23.205831790538902</v>
       </c>
       <c r="E76" s="8">
-        <v>18.829710357548414</v>
+        <v>49.4624465420127</v>
       </c>
       <c r="F76" s="8">
-        <v>0.62700849999999997</v>
+        <v>1.57411375</v>
       </c>
       <c r="G76" s="8">
-        <v>-0.33165162163020123</v>
+        <v>-1.560405679460718</v>
       </c>
       <c r="H76" s="8">
-        <v>4.933828923826284</v>
+        <v>11.430485837178477</v>
       </c>
       <c r="I76" s="8">
-        <v>3.8170000000000002</v>
+        <v>4.327</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C77" s="8">
-        <v>2.386304</v>
+        <v>5.6755789999999999</v>
       </c>
       <c r="D77" s="11">
-        <v>-25.298547291521309</v>
+        <v>-21.792215917181593</v>
       </c>
       <c r="E77" s="8">
-        <v>28.947319595966892</v>
+        <v>67.267485604681823</v>
       </c>
       <c r="F77" s="8">
-        <v>0.96525075000000005</v>
+        <v>2.6374545</v>
       </c>
       <c r="G77" s="8">
-        <v>-0.27194060419857169</v>
+        <v>-0.91289631787740855</v>
       </c>
       <c r="H77" s="8">
-        <v>7.413621955214146</v>
+        <v>18.675748686039249</v>
       </c>
       <c r="I77" s="8">
-        <v>3.9039999999999999</v>
+        <v>3.6019999999999999</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C78" s="8">
-        <v>7.6152749999999996</v>
+        <v>3.8125697500000002</v>
       </c>
       <c r="D78" s="11">
-        <v>-25.732896740956409</v>
+        <v>-23.095778996863721</v>
       </c>
       <c r="E78" s="8">
-        <v>90.984209695175196</v>
+        <v>45.727064390053997</v>
       </c>
       <c r="F78" s="8">
-        <v>3.50915775</v>
+        <v>1.5458248750000001</v>
       </c>
       <c r="G78" s="8">
-        <v>-1.1615637497241138</v>
+        <v>0.47209794551692608</v>
       </c>
       <c r="H78" s="8">
-        <v>24.702444077116027</v>
+        <v>11.483077140860548</v>
       </c>
       <c r="I78" s="8">
-        <v>3.6829999999999998</v>
+        <v>3.98</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C79" s="8">
-        <v>4.1858392499999999</v>
+        <v>2.1744599999999998</v>
       </c>
       <c r="D79" s="11">
-        <v>-23.205831790538902</v>
+        <v>-25.18327736825465</v>
       </c>
       <c r="E79" s="8">
-        <v>49.4624465420127</v>
+        <v>25.923758954464198</v>
       </c>
       <c r="F79" s="8">
-        <v>1.57411375</v>
+        <v>0.89151262499999995</v>
       </c>
       <c r="G79" s="8">
-        <v>-1.560405679460718</v>
+        <v>-0.32070061787816573</v>
       </c>
       <c r="H79" s="8">
-        <v>11.430485837178477</v>
+        <v>6.5134269162660861</v>
       </c>
       <c r="I79" s="8">
-        <v>4.327</v>
+        <v>3.98</v>
       </c>
       <c r="J79" s="8"/>
       <c r="K79" s="8"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C80" s="8">
-        <v>5.6755789999999999</v>
+        <v>4.4142669999999997</v>
       </c>
       <c r="D80" s="11">
-        <v>-21.792215917181593</v>
+        <v>-21.544695399470086</v>
       </c>
       <c r="E80" s="8">
-        <v>67.267485604681823</v>
+        <v>52.307294165541805</v>
       </c>
       <c r="F80" s="8">
-        <v>2.6374545</v>
+        <v>2.0034467500000002</v>
       </c>
       <c r="G80" s="8">
-        <v>-0.91289631787740855</v>
+        <v>-1.2418707027521891</v>
       </c>
       <c r="H80" s="8">
-        <v>18.675748686039249</v>
+        <v>13.941878351023124</v>
       </c>
       <c r="I80" s="8">
-        <v>3.6019999999999999</v>
+        <v>3.7519999999999998</v>
       </c>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C81" s="8">
-        <v>3.8125697500000002</v>
+        <v>2.6094884999999999</v>
       </c>
       <c r="D81" s="11">
-        <v>-23.095778996863721</v>
+        <v>-25.677802130816769</v>
       </c>
       <c r="E81" s="8">
-        <v>45.727064390053997</v>
+        <v>31.012638516248273</v>
       </c>
       <c r="F81" s="8">
-        <v>1.5458248750000001</v>
+        <v>1.1081622499999999</v>
       </c>
       <c r="G81" s="8">
-        <v>0.47209794551692608</v>
+        <v>-1.1860859516713773</v>
       </c>
       <c r="H81" s="8">
-        <v>11.483077140860548</v>
+        <v>7.9616602827366529</v>
       </c>
       <c r="I81" s="8">
-        <v>3.98</v>
+        <v>3.8959999999999999</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C82" s="8">
-        <v>2.1744599999999998</v>
-      </c>
-      <c r="D82" s="11">
-        <v>-25.18327736825465</v>
-      </c>
-      <c r="E82" s="8">
-        <v>25.923758954464198</v>
-      </c>
-      <c r="F82" s="8">
-        <v>0.89151262499999995</v>
-      </c>
-      <c r="G82" s="8">
-        <v>-0.32070061787816573</v>
-      </c>
-      <c r="H82" s="8">
-        <v>6.5134269162660861</v>
-      </c>
-      <c r="I82" s="8">
-        <v>3.98</v>
-      </c>
+      <c r="A82" s="11"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C83" s="8">
-        <v>4.4142669999999997</v>
+        <v>2.5927695000000002</v>
       </c>
       <c r="D83" s="11">
-        <v>-21.544695399470086</v>
+        <v>-22.39897712807754</v>
       </c>
       <c r="E83" s="8">
-        <v>52.307294165541805</v>
+        <v>31.098291479601922</v>
       </c>
       <c r="F83" s="8">
-        <v>2.0034467500000002</v>
+        <v>1.092631125</v>
       </c>
       <c r="G83" s="8">
-        <v>-1.2418707027521891</v>
+        <v>0.34330798080493108</v>
       </c>
       <c r="H83" s="8">
-        <v>13.941878351023124</v>
+        <v>7.8807132037398144</v>
       </c>
       <c r="I83" s="8">
-        <v>3.7519999999999998</v>
+        <v>3.9460000000000002</v>
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C84" s="8">
-        <v>2.6094884999999999</v>
+        <v>5.3232730000000004</v>
       </c>
       <c r="D84" s="11">
-        <v>-25.677802130816769</v>
+        <v>-21.587139849794891</v>
       </c>
       <c r="E84" s="8">
-        <v>31.012638516248273</v>
+        <v>63.257597889558113</v>
       </c>
       <c r="F84" s="8">
-        <v>1.1081622499999999</v>
+        <v>2.3595925000000002</v>
       </c>
       <c r="G84" s="8">
-        <v>-1.1860859516713773</v>
+        <v>-0.34814713117472418</v>
       </c>
       <c r="H84" s="8">
-        <v>7.9616602827366529</v>
+        <v>16.189000946651493</v>
       </c>
       <c r="I84" s="8">
-        <v>3.8959999999999999</v>
+        <v>3.907</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
+      <c r="A85" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" s="8">
+        <v>6.2965594999999999</v>
+      </c>
+      <c r="D85" s="11">
+        <v>-23.779637766696524</v>
+      </c>
+      <c r="E85" s="8">
+        <v>74.459028942652324</v>
+      </c>
+      <c r="F85" s="8">
+        <v>2.3650207499999998</v>
+      </c>
+      <c r="G85" s="8">
+        <v>-0.11373904305646998</v>
+      </c>
+      <c r="H85" s="8">
+        <v>16.165913219008214</v>
+      </c>
+      <c r="I85" s="8">
+        <v>4.6059999999999999</v>
+      </c>
       <c r="J85" s="8"/>
       <c r="K85" s="8"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C86" s="8">
-        <v>2.5927695000000002</v>
-      </c>
-      <c r="D86" s="11">
-        <v>-22.39897712807754</v>
-      </c>
-      <c r="E86" s="8">
-        <v>31.098291479601922</v>
-      </c>
-      <c r="F86" s="8">
-        <v>1.092631125</v>
-      </c>
-      <c r="G86" s="8">
-        <v>0.34330798080493108</v>
-      </c>
-      <c r="H86" s="8">
-        <v>7.8807132037398144</v>
-      </c>
-      <c r="I86" s="8">
-        <v>3.9460000000000002</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
       <c r="J86" s="8"/>
       <c r="K86" s="8"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C87" s="8">
-        <v>5.3232730000000004</v>
-      </c>
-      <c r="D87" s="11">
-        <v>-21.587139849794891</v>
+        <v>2.0100994999999999</v>
+      </c>
+      <c r="D87" s="8">
+        <v>-26.11510649612509</v>
       </c>
       <c r="E87" s="8">
-        <v>63.257597889558113</v>
+        <v>23.422244799920886</v>
       </c>
       <c r="F87" s="8">
-        <v>2.3595925000000002</v>
+        <v>0.73620093750000004</v>
       </c>
       <c r="G87" s="8">
-        <v>-0.34814713117472418</v>
+        <v>1.9061262501519416</v>
       </c>
       <c r="H87" s="8">
-        <v>16.189000946651493</v>
+        <v>5.5925924399783513</v>
       </c>
       <c r="I87" s="8">
-        <v>3.907</v>
+        <v>4.1879999999999997</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="8"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C88" s="8">
-        <v>6.2965594999999999</v>
-      </c>
-      <c r="D88" s="11">
-        <v>-23.779637766696524</v>
+        <v>1.82299575</v>
+      </c>
+      <c r="D88" s="8">
+        <v>-26.212406794108187</v>
       </c>
       <c r="E88" s="8">
-        <v>74.459028942652324</v>
+        <v>21.318905122663953</v>
       </c>
       <c r="F88" s="8">
-        <v>2.3650207499999998</v>
+        <v>0.7623966875</v>
       </c>
       <c r="G88" s="8">
-        <v>-0.11373904305646998</v>
+        <v>2.1333086916333963</v>
       </c>
       <c r="H88" s="8">
-        <v>16.165913219008214</v>
+        <v>5.7508962553141636</v>
       </c>
       <c r="I88" s="8">
-        <v>4.6059999999999999</v>
+        <v>3.7077</v>
       </c>
       <c r="J88" s="8"/>
       <c r="K88" s="8"/>
@@ -4535,920 +4565,882 @@
       <c r="A89" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
+      <c r="B89" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C89" s="8">
+        <v>4.5792444999999997</v>
+      </c>
+      <c r="D89" s="8">
+        <v>-25.31304278625975</v>
+      </c>
+      <c r="E89" s="8">
+        <v>54.205932986319766</v>
+      </c>
+      <c r="F89" s="8">
+        <v>2.0072286250000002</v>
+      </c>
+      <c r="G89" s="8">
+        <v>0.65697709499099699</v>
+      </c>
+      <c r="H89" s="8">
+        <v>14.269305780156079</v>
+      </c>
+      <c r="I89" s="8">
+        <v>3.7989999999999999</v>
+      </c>
       <c r="J89" s="8"/>
       <c r="K89" s="8"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C90" s="8">
-        <v>2.0100994999999999</v>
+        <v>5.2121959999999996</v>
       </c>
       <c r="D90" s="8">
-        <v>-26.11510649612509</v>
+        <v>-25.703458411062815</v>
       </c>
       <c r="E90" s="8">
-        <v>23.422244799920886</v>
+        <v>62.587928319211265</v>
       </c>
       <c r="F90" s="8">
-        <v>0.73620093750000004</v>
+        <v>2.1780655000000002</v>
       </c>
       <c r="G90" s="8">
-        <v>1.9061262501519416</v>
+        <v>1.7580788425698224</v>
       </c>
       <c r="H90" s="8">
-        <v>5.5925924399783513</v>
+        <v>15.80736864208734</v>
       </c>
       <c r="I90" s="8">
-        <v>4.1879999999999997</v>
+        <v>3.9590000000000001</v>
       </c>
       <c r="J90" s="8"/>
       <c r="K90" s="8"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C91" s="8">
-        <v>1.82299575</v>
+        <v>7.0732569999999999</v>
       </c>
       <c r="D91" s="8">
-        <v>-26.212406794108187</v>
+        <v>-25.05553291740932</v>
       </c>
       <c r="E91" s="8">
-        <v>21.318905122663953</v>
+        <v>84.565415262572486</v>
       </c>
       <c r="F91" s="8">
-        <v>0.7623966875</v>
+        <v>3.1160480000000002</v>
       </c>
       <c r="G91" s="8">
-        <v>2.1333086916333963</v>
+        <v>2.3078146970115574</v>
       </c>
       <c r="H91" s="8">
-        <v>5.7508962553141636</v>
+        <v>21.144868710636334</v>
       </c>
       <c r="I91" s="8">
-        <v>3.7077</v>
+        <v>3.9990000000000001</v>
       </c>
       <c r="J91" s="8"/>
       <c r="K91" s="8"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C92" s="8">
-        <v>4.5792444999999997</v>
+        <v>3.3093715000000001</v>
       </c>
       <c r="D92" s="8">
-        <v>-25.31304278625975</v>
+        <v>-26.377674109670743</v>
       </c>
       <c r="E92" s="8">
-        <v>54.205932986319766</v>
+        <v>39.058945698283637</v>
       </c>
       <c r="F92" s="8">
-        <v>2.0072286250000002</v>
+        <v>1.2830263749999999</v>
       </c>
       <c r="G92" s="8">
-        <v>0.65697709499099699</v>
+        <v>1.4103281879683582</v>
       </c>
       <c r="H92" s="8">
-        <v>14.269305780156079</v>
+        <v>9.1245093668162891</v>
       </c>
       <c r="I92" s="8">
-        <v>3.7989999999999999</v>
+        <v>4.28</v>
       </c>
       <c r="J92" s="8"/>
       <c r="K92" s="8"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C93" s="8">
-        <v>5.2121959999999996</v>
+        <v>2.1929460000000001</v>
       </c>
       <c r="D93" s="8">
-        <v>-25.703458411062815</v>
+        <v>-25.735096296503837</v>
       </c>
       <c r="E93" s="8">
-        <v>62.587928319211265</v>
+        <v>26.079879645154893</v>
       </c>
       <c r="F93" s="8">
-        <v>2.1780655000000002</v>
+        <v>0.95398918749999995</v>
       </c>
       <c r="G93" s="8">
-        <v>1.7580788425698224</v>
+        <v>0.84756565041286369</v>
       </c>
       <c r="H93" s="8">
-        <v>15.80736864208734</v>
+        <v>6.9290391653542951</v>
       </c>
       <c r="I93" s="8">
-        <v>3.9590000000000001</v>
+        <v>3.7639999999999998</v>
       </c>
       <c r="J93" s="8"/>
       <c r="K93" s="8"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C94" s="8">
-        <v>7.0732569999999999</v>
-      </c>
-      <c r="D94" s="8">
-        <v>-25.05553291740932</v>
-      </c>
-      <c r="E94" s="8">
-        <v>84.565415262572486</v>
-      </c>
-      <c r="F94" s="8">
-        <v>3.1160480000000002</v>
-      </c>
-      <c r="G94" s="8">
-        <v>2.3078146970115574</v>
-      </c>
-      <c r="H94" s="8">
-        <v>21.144868710636334</v>
-      </c>
-      <c r="I94" s="8">
-        <v>3.9990000000000001</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
       <c r="J94" s="8"/>
       <c r="K94" s="8"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C95" s="8">
-        <v>3.3093715000000001</v>
+        <v>5.3673869999999999</v>
       </c>
       <c r="D95" s="8">
-        <v>-26.377674109670743</v>
+        <v>-24.929629229021248</v>
       </c>
       <c r="E95" s="8">
-        <v>39.058945698283637</v>
+        <v>64.427285785014348</v>
       </c>
       <c r="F95" s="8">
-        <v>1.2830263749999999</v>
+        <v>2.0023733749999999</v>
       </c>
       <c r="G95" s="8">
-        <v>1.4103281879683582</v>
+        <v>-0.50768494930743979</v>
       </c>
       <c r="H95" s="8">
-        <v>9.1245093668162891</v>
+        <v>14.697766949424105</v>
       </c>
       <c r="I95" s="8">
-        <v>4.28</v>
+        <v>4.383</v>
       </c>
       <c r="J95" s="8"/>
       <c r="K95" s="8"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C96" s="8">
-        <v>2.1929460000000001</v>
+        <v>6.9515500000000001</v>
       </c>
       <c r="D96" s="8">
-        <v>-25.735096296503837</v>
+        <v>-22.852615091011618</v>
       </c>
       <c r="E96" s="8">
-        <v>26.079879645154893</v>
+        <v>83.521690265263743</v>
       </c>
       <c r="F96" s="8">
-        <v>0.95398918749999995</v>
+        <v>2.7440037500000001</v>
       </c>
       <c r="G96" s="8">
-        <v>0.84756565041286369</v>
+        <v>0.92589027234111332</v>
       </c>
       <c r="H96" s="8">
-        <v>6.9290391653542951</v>
+        <v>19.626528935302218</v>
       </c>
       <c r="I96" s="8">
-        <v>3.7639999999999998</v>
+        <v>4.2549999999999999</v>
       </c>
       <c r="J96" s="8"/>
       <c r="K96" s="8"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B97" s="8"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
+      <c r="B97" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" s="8">
+        <v>2.4511319999999999</v>
+      </c>
+      <c r="D97" s="8">
+        <v>-22.546143132935846</v>
+      </c>
+      <c r="E97" s="8">
+        <v>29.6366060549392</v>
+      </c>
+      <c r="F97" s="8">
+        <v>1.1318680000000001</v>
+      </c>
+      <c r="G97" s="8">
+        <v>-2.2503341390035727</v>
+      </c>
+      <c r="H97" s="8">
+        <v>8.4945892002841106</v>
+      </c>
+      <c r="I97" s="8">
+        <v>3.4889999999999999</v>
+      </c>
       <c r="J97" s="8"/>
       <c r="K97" s="8"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C98" s="8">
-        <v>5.3673869999999999</v>
+        <v>6.3285340000000003</v>
       </c>
       <c r="D98" s="8">
-        <v>-24.929629229021248</v>
+        <v>-23.450232299011287</v>
       </c>
       <c r="E98" s="8">
-        <v>64.427285785014348</v>
+        <v>77.217160070851904</v>
       </c>
       <c r="F98" s="8">
-        <v>2.0023733749999999</v>
+        <v>3.19859625</v>
       </c>
       <c r="G98" s="8">
-        <v>-0.50768494930743979</v>
+        <v>-0.87107834429436148</v>
       </c>
       <c r="H98" s="8">
-        <v>14.697766949424105</v>
+        <v>22.638790346326616</v>
       </c>
       <c r="I98" s="8">
-        <v>4.383</v>
+        <v>3.41</v>
       </c>
       <c r="J98" s="8"/>
       <c r="K98" s="8"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C99" s="8">
-        <v>6.9515500000000001</v>
+        <v>3.3373987500000002</v>
       </c>
       <c r="D99" s="8">
-        <v>-22.852615091011618</v>
+        <v>-24.588064727422083</v>
       </c>
       <c r="E99" s="8">
-        <v>83.521690265263743</v>
+        <v>39.384161045360152</v>
       </c>
       <c r="F99" s="8">
-        <v>2.7440037500000001</v>
+        <v>1.464306375</v>
       </c>
       <c r="G99" s="8">
-        <v>0.92589027234111332</v>
+        <v>0.32491864983228536</v>
       </c>
       <c r="H99" s="8">
-        <v>19.626528935302218</v>
+        <v>10.69040882478172</v>
       </c>
       <c r="I99" s="8">
-        <v>4.2549999999999999</v>
+        <v>3.6840000000000002</v>
       </c>
       <c r="J99" s="8"/>
       <c r="K99" s="8"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C100" s="8">
-        <v>2.4511319999999999</v>
+        <v>6.9879825000000002</v>
       </c>
       <c r="D100" s="8">
-        <v>-22.546143132935846</v>
+        <v>-24.918359887644062</v>
       </c>
       <c r="E100" s="8">
-        <v>29.6366060549392</v>
+        <v>85.137602405917036</v>
       </c>
       <c r="F100" s="8">
-        <v>1.1318680000000001</v>
+        <v>3.3323957499999999</v>
       </c>
       <c r="G100" s="8">
-        <v>-2.2503341390035727</v>
+        <v>-0.19423757138650077</v>
       </c>
       <c r="H100" s="8">
-        <v>8.4945892002841106</v>
+        <v>23.609994925298448</v>
       </c>
       <c r="I100" s="8">
-        <v>3.4889999999999999</v>
+        <v>3.6059999999999999</v>
       </c>
       <c r="J100" s="8"/>
       <c r="K100" s="8"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C101" s="8">
-        <v>6.3285340000000003</v>
+        <v>3.2461562499999999</v>
       </c>
       <c r="D101" s="8">
-        <v>-23.450232299011287</v>
+        <v>-23.76004930524271</v>
       </c>
       <c r="E101" s="8">
-        <v>77.217160070851904</v>
+        <v>38.68255136407614</v>
       </c>
       <c r="F101" s="8">
-        <v>3.19859625</v>
+        <v>1.570607125</v>
       </c>
       <c r="G101" s="8">
-        <v>-0.87107834429436148</v>
+        <v>0.45066098277533162</v>
       </c>
       <c r="H101" s="8">
-        <v>22.638790346326616</v>
+        <v>11.395248766713094</v>
       </c>
       <c r="I101" s="8">
-        <v>3.41</v>
+        <v>3.395</v>
       </c>
       <c r="J101" s="8"/>
       <c r="K101" s="8"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C102" s="8">
-        <v>3.3373987500000002</v>
+        <v>5.5487830000000002</v>
       </c>
       <c r="D102" s="8">
-        <v>-24.588064727422083</v>
+        <v>-23.874434892722999</v>
       </c>
       <c r="E102" s="8">
-        <v>39.384161045360152</v>
+        <v>68.210702510969242</v>
       </c>
       <c r="F102" s="8">
-        <v>1.464306375</v>
+        <v>2.3597475000000001</v>
       </c>
       <c r="G102" s="8">
-        <v>0.32491864983228536</v>
+        <v>-1.2265385360256331</v>
       </c>
       <c r="H102" s="8">
-        <v>10.69040882478172</v>
+        <v>17.026126726601884</v>
       </c>
       <c r="I102" s="8">
-        <v>3.6840000000000002</v>
+        <v>4.0049999999999999</v>
       </c>
       <c r="J102" s="8"/>
       <c r="K102" s="8"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C103" s="8">
-        <v>6.9879825000000002</v>
+        <v>7.1157510000000004</v>
       </c>
       <c r="D103" s="8">
-        <v>-24.918359887644062</v>
+        <v>-24.942868803843488</v>
       </c>
       <c r="E103" s="8">
-        <v>85.137602405917036</v>
+        <v>85.813263476090668</v>
       </c>
       <c r="F103" s="8">
-        <v>3.3323957499999999</v>
+        <v>3.096374</v>
       </c>
       <c r="G103" s="8">
-        <v>-0.19423757138650077</v>
+        <v>-0.23787629084339623</v>
       </c>
       <c r="H103" s="8">
-        <v>23.609994925298448</v>
+        <v>21.199168658163533</v>
       </c>
       <c r="I103" s="8">
-        <v>3.6059999999999999</v>
+        <v>4.048</v>
       </c>
       <c r="J103" s="8"/>
       <c r="K103" s="8"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C104" s="8">
-        <v>3.2461562499999999</v>
+        <v>2.7798667500000001</v>
       </c>
       <c r="D104" s="8">
-        <v>-23.76004930524271</v>
+        <v>-23.345349296772966</v>
       </c>
       <c r="E104" s="8">
-        <v>38.68255136407614</v>
+        <v>33.180255321124271</v>
       </c>
       <c r="F104" s="8">
-        <v>1.570607125</v>
+        <v>1.3053376249999999</v>
       </c>
       <c r="G104" s="8">
-        <v>0.45066098277533162</v>
+        <v>-0.68664882868332167</v>
       </c>
       <c r="H104" s="8">
-        <v>11.395248766713094</v>
+        <v>9.2950588852472524</v>
       </c>
       <c r="I104" s="8">
-        <v>3.395</v>
+        <v>3.57</v>
       </c>
       <c r="J104" s="8"/>
       <c r="K104" s="8"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C105" s="8">
-        <v>5.5487830000000002</v>
+        <v>6.4766044999999997</v>
       </c>
       <c r="D105" s="8">
-        <v>-23.874434892722999</v>
+        <v>-22.471431223222289</v>
       </c>
       <c r="E105" s="8">
-        <v>68.210702510969242</v>
+        <v>78.436889084848119</v>
       </c>
       <c r="F105" s="8">
-        <v>2.3597475000000001</v>
+        <v>2.7201767499999998</v>
       </c>
       <c r="G105" s="8">
-        <v>-1.2265385360256331</v>
+        <v>0.99498358494130135</v>
       </c>
       <c r="H105" s="8">
-        <v>17.026126726601884</v>
+        <v>18.74395417062879</v>
       </c>
       <c r="I105" s="8">
-        <v>4.0049999999999999</v>
+        <v>4.18</v>
       </c>
       <c r="J105" s="8"/>
       <c r="K105" s="8"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C106" s="8">
-        <v>7.1157510000000004</v>
-      </c>
-      <c r="D106" s="8">
-        <v>-24.942868803843488</v>
-      </c>
-      <c r="E106" s="8">
-        <v>85.813263476090668</v>
-      </c>
-      <c r="F106" s="8">
-        <v>3.096374</v>
-      </c>
-      <c r="G106" s="8">
-        <v>-0.23787629084339623</v>
-      </c>
-      <c r="H106" s="8">
-        <v>21.199168658163533</v>
-      </c>
-      <c r="I106" s="8">
-        <v>4.048</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B106" s="8"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E106" s="8"/>
+      <c r="F106" s="8"/>
+      <c r="G106" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
       <c r="J106" s="8"/>
       <c r="K106" s="8"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C107" s="8">
-        <v>2.7798667500000001</v>
+        <v>8.2100884999999995</v>
       </c>
       <c r="D107" s="8">
-        <v>-23.345349296772966</v>
+        <v>-26.161022198695779</v>
       </c>
       <c r="E107" s="8">
-        <v>33.180255321124271</v>
+        <v>99.141529629633879</v>
       </c>
       <c r="F107" s="8">
-        <v>1.3053376249999999</v>
+        <v>3.86983575</v>
       </c>
       <c r="G107" s="8">
-        <v>-0.68664882868332167</v>
+        <v>-0.1504427370072825</v>
       </c>
       <c r="H107" s="8">
-        <v>9.2950588852472524</v>
+        <v>27.174764232191528</v>
       </c>
       <c r="I107" s="8">
-        <v>3.57</v>
+        <v>3.6480000000000001</v>
       </c>
       <c r="J107" s="8"/>
       <c r="K107" s="8"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C108" s="8">
-        <v>6.4766044999999997</v>
+        <v>2.6094244999999998</v>
       </c>
       <c r="D108" s="8">
-        <v>-22.471431223222289</v>
+        <v>-25.010873944145505</v>
       </c>
       <c r="E108" s="8">
-        <v>78.436889084848119</v>
+        <v>30.856728755945873</v>
       </c>
       <c r="F108" s="8">
-        <v>2.7201767499999998</v>
+        <v>1.0045558125</v>
       </c>
       <c r="G108" s="8">
-        <v>0.99498358494130135</v>
+        <v>-1.4183073502052268</v>
       </c>
       <c r="H108" s="8">
-        <v>18.74395417062879</v>
+        <v>7.5703686896631286</v>
       </c>
       <c r="I108" s="8">
-        <v>4.18</v>
+        <v>4.0759999999999996</v>
       </c>
       <c r="J108" s="8"/>
       <c r="K108" s="8"/>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H109" s="8"/>
-      <c r="I109" s="8"/>
+        <v>134</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C109" s="8">
+        <v>11.880023</v>
+      </c>
+      <c r="D109" s="8">
+        <v>-26.254260051457784</v>
+      </c>
+      <c r="E109" s="8">
+        <v>146.33151906577959</v>
+      </c>
+      <c r="F109" s="8">
+        <v>6.2927710000000001</v>
+      </c>
+      <c r="G109" s="8">
+        <v>-0.4115480754071299</v>
+      </c>
+      <c r="H109" s="8">
+        <v>42.588534857261415</v>
+      </c>
+      <c r="I109" s="8">
+        <v>3.4359999999999999</v>
+      </c>
       <c r="J109" s="8"/>
       <c r="K109" s="8"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C110" s="8">
-        <v>8.2100884999999995</v>
+        <v>2.9896362500000002</v>
       </c>
       <c r="D110" s="8">
-        <v>-26.161022198695779</v>
+        <v>-24.481683134558086</v>
       </c>
       <c r="E110" s="8">
-        <v>99.141529629633879</v>
+        <v>36.535104684358508</v>
       </c>
       <c r="F110" s="8">
-        <v>3.86983575</v>
+        <v>1.380250875</v>
       </c>
       <c r="G110" s="8">
-        <v>-0.1504427370072825</v>
+        <v>-6.0148631173672085E-2</v>
       </c>
       <c r="H110" s="8">
-        <v>27.174764232191528</v>
+        <v>10.23877481440114</v>
       </c>
       <c r="I110" s="8">
-        <v>3.6480000000000001</v>
+        <v>3.5680000000000001</v>
       </c>
       <c r="J110" s="8"/>
       <c r="K110" s="8"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C111" s="8">
-        <v>2.6094244999999998</v>
+        <v>3.0724897499999999</v>
       </c>
       <c r="D111" s="8">
-        <v>-25.010873944145505</v>
+        <v>-25.3057828391808</v>
       </c>
       <c r="E111" s="8">
-        <v>30.856728755945873</v>
+        <v>36.59366970466921</v>
       </c>
       <c r="F111" s="8">
-        <v>1.0045558125</v>
+        <v>1.3404756250000001</v>
       </c>
       <c r="G111" s="8">
-        <v>-1.4183073502052268</v>
+        <v>0.74845027286927324</v>
       </c>
       <c r="H111" s="8">
-        <v>7.5703686896631286</v>
+        <v>9.8570528929136341</v>
       </c>
       <c r="I111" s="8">
-        <v>4.0759999999999996</v>
+        <v>3.7120000000000002</v>
       </c>
       <c r="J111" s="8"/>
       <c r="K111" s="8"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C112" s="8">
-        <v>11.880023</v>
+        <v>3.1625865000000002</v>
       </c>
       <c r="D112" s="8">
-        <v>-26.254260051457784</v>
+        <v>-26.324388683318286</v>
       </c>
       <c r="E112" s="8">
-        <v>146.33151906577959</v>
+        <v>37.709720659218164</v>
       </c>
       <c r="F112" s="8">
-        <v>6.2927710000000001</v>
+        <v>1.192895</v>
       </c>
       <c r="G112" s="8">
-        <v>-0.4115480754071299</v>
+        <v>-1.0585684395795425</v>
       </c>
       <c r="H112" s="8">
-        <v>42.588534857261415</v>
+        <v>8.9071471206862682</v>
       </c>
       <c r="I112" s="8">
-        <v>3.4359999999999999</v>
+        <v>4.2320000000000002</v>
       </c>
       <c r="J112" s="8"/>
       <c r="K112" s="8"/>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C113" s="8">
-        <v>2.9896362500000002</v>
+        <v>8.4342679999999994</v>
       </c>
       <c r="D113" s="8">
-        <v>-24.481683134558086</v>
+        <v>-26.148350817574883</v>
       </c>
       <c r="E113" s="8">
-        <v>36.535104684358508</v>
+        <v>101.43023203024528</v>
       </c>
       <c r="F113" s="8">
-        <v>1.380250875</v>
+        <v>4.0331112500000001</v>
       </c>
       <c r="G113" s="8">
-        <v>-6.0148631173672085E-2</v>
+        <v>-0.42874158277630303</v>
       </c>
       <c r="H113" s="8">
-        <v>10.23877481440114</v>
+        <v>28.017485677390948</v>
       </c>
       <c r="I113" s="8">
-        <v>3.5680000000000001</v>
+        <v>3.62</v>
       </c>
       <c r="J113" s="8"/>
       <c r="K113" s="8"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="11" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C114" s="8">
-        <v>3.0724897499999999</v>
+        <v>1.4996242500000001</v>
       </c>
       <c r="D114" s="8">
-        <v>-25.3057828391808</v>
+        <v>-25.471423471265751</v>
       </c>
       <c r="E114" s="8">
-        <v>36.59366970466921</v>
+        <v>18.216155758809492</v>
       </c>
       <c r="F114" s="8">
-        <v>1.3404756250000001</v>
+        <v>0.62575312500000002</v>
       </c>
       <c r="G114" s="8">
-        <v>0.74845027286927324</v>
+        <v>0.86046188903208365</v>
       </c>
       <c r="H114" s="8">
-        <v>9.8570528929136341</v>
+        <v>4.7065048355789472</v>
       </c>
       <c r="I114" s="8">
-        <v>3.7120000000000002</v>
+        <v>3.8698999999999999</v>
       </c>
       <c r="J114" s="8"/>
       <c r="K114" s="8"/>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C115" s="8">
-        <v>3.1625865000000002</v>
+        <v>7.4181629999999998</v>
       </c>
       <c r="D115" s="8">
-        <v>-26.324388683318286</v>
+        <v>-25.868999200059761</v>
       </c>
       <c r="E115" s="8">
-        <v>37.709720659218164</v>
+        <v>90.463728377949593</v>
       </c>
       <c r="F115" s="8">
-        <v>1.192895</v>
+        <v>3.6572809999999998</v>
       </c>
       <c r="G115" s="8">
-        <v>-1.0585684395795425</v>
+        <v>-0.8499233803708417</v>
       </c>
       <c r="H115" s="8">
-        <v>8.9071471206862682</v>
+        <v>24.978902920633484</v>
       </c>
       <c r="I115" s="8">
-        <v>4.2320000000000002</v>
+        <v>3.6219999999999999</v>
       </c>
       <c r="J115" s="8"/>
       <c r="K115" s="8"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="11" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C116" s="8">
-        <v>8.4342679999999994</v>
+        <v>6.1446845000000003</v>
       </c>
       <c r="D116" s="8">
-        <v>-26.148350817574883</v>
+        <v>-25.645271591624688</v>
       </c>
       <c r="E116" s="8">
-        <v>101.43023203024528</v>
+        <v>74.707293997793371</v>
       </c>
       <c r="F116" s="8">
-        <v>4.0331112500000001</v>
+        <v>2.9235764999999998</v>
       </c>
       <c r="G116" s="8">
-        <v>-0.42874158277630303</v>
+        <v>-0.42562981849716297</v>
       </c>
       <c r="H116" s="8">
-        <v>28.017485677390948</v>
+        <v>20.252847000499983</v>
       </c>
       <c r="I116" s="8">
-        <v>3.62</v>
+        <v>3.6890000000000001</v>
       </c>
       <c r="J116" s="8"/>
       <c r="K116" s="8"/>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A117" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C117" s="8">
-        <v>1.4996242500000001</v>
-      </c>
-      <c r="D117" s="8">
-        <v>-25.471423471265751</v>
-      </c>
-      <c r="E117" s="8">
-        <v>18.216155758809492</v>
-      </c>
-      <c r="F117" s="8">
-        <v>0.62575312500000002</v>
-      </c>
-      <c r="G117" s="8">
-        <v>0.86046188903208365</v>
-      </c>
-      <c r="H117" s="8">
-        <v>4.7065048355789472</v>
-      </c>
-      <c r="I117" s="8">
-        <v>3.8698999999999999</v>
-      </c>
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="8"/>
+      <c r="F117" s="8"/>
+      <c r="G117" s="11"/>
+      <c r="H117" s="8"/>
+      <c r="I117" s="8"/>
       <c r="J117" s="8"/>
       <c r="K117" s="8"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B118" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C118" s="8">
-        <v>7.4181629999999998</v>
-      </c>
-      <c r="D118" s="8">
-        <v>-25.868999200059761</v>
-      </c>
-      <c r="E118" s="8">
-        <v>90.463728377949593</v>
-      </c>
-      <c r="F118" s="8">
-        <v>3.6572809999999998</v>
-      </c>
-      <c r="G118" s="8">
-        <v>-0.8499233803708417</v>
-      </c>
-      <c r="H118" s="8">
-        <v>24.978902920633484</v>
-      </c>
-      <c r="I118" s="8">
-        <v>3.6219999999999999</v>
-      </c>
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8"/>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
       <c r="J118" s="8"/>
       <c r="K118" s="8"/>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A119" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B119" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C119" s="8">
-        <v>6.1446845000000003</v>
-      </c>
-      <c r="D119" s="8">
-        <v>-25.645271591624688</v>
-      </c>
-      <c r="E119" s="8">
-        <v>74.707293997793371</v>
-      </c>
-      <c r="F119" s="8">
-        <v>2.9235764999999998</v>
-      </c>
-      <c r="G119" s="8">
-        <v>-0.42562981849716297</v>
-      </c>
-      <c r="H119" s="8">
-        <v>20.252847000499983</v>
-      </c>
-      <c r="I119" s="8">
-        <v>3.6890000000000001</v>
-      </c>
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8"/>
+      <c r="F119" s="8"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8"/>
+      <c r="I119" s="8"/>
       <c r="J119" s="8"/>
       <c r="K119" s="8"/>
     </row>
@@ -5456,10 +5448,10 @@
       <c r="A120" s="8"/>
       <c r="B120" s="8"/>
       <c r="C120" s="8"/>
-      <c r="D120" s="11"/>
+      <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
-      <c r="G120" s="11"/>
+      <c r="G120" s="8"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
@@ -5557,10 +5549,10 @@
       <c r="K127" s="8"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
+      <c r="A128" s="11"/>
       <c r="B128" s="8"/>
       <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
+      <c r="D128" s="29"/>
       <c r="E128" s="8"/>
       <c r="F128" s="8"/>
       <c r="G128" s="8"/>
@@ -5570,10 +5562,10 @@
       <c r="K128" s="8"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A129" s="8"/>
+      <c r="A129" s="11"/>
       <c r="B129" s="8"/>
       <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
+      <c r="D129" s="29"/>
       <c r="E129" s="8"/>
       <c r="F129" s="8"/>
       <c r="G129" s="8"/>
@@ -5583,10 +5575,10 @@
       <c r="K129" s="8"/>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A130" s="8"/>
+      <c r="A130" s="11"/>
       <c r="B130" s="8"/>
       <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
+      <c r="D130" s="29"/>
       <c r="E130" s="8"/>
       <c r="F130" s="8"/>
       <c r="G130" s="8"/>
@@ -5716,7 +5708,7 @@
       <c r="A140" s="11"/>
       <c r="B140" s="8"/>
       <c r="C140" s="8"/>
-      <c r="D140" s="29"/>
+      <c r="D140" s="8"/>
       <c r="E140" s="8"/>
       <c r="F140" s="8"/>
       <c r="G140" s="8"/>
@@ -5729,7 +5721,7 @@
       <c r="A141" s="11"/>
       <c r="B141" s="8"/>
       <c r="C141" s="8"/>
-      <c r="D141" s="29"/>
+      <c r="D141" s="8"/>
       <c r="E141" s="8"/>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
@@ -5742,7 +5734,7 @@
       <c r="A142" s="11"/>
       <c r="B142" s="8"/>
       <c r="C142" s="8"/>
-      <c r="D142" s="29"/>
+      <c r="D142" s="8"/>
       <c r="E142" s="8"/>
       <c r="F142" s="8"/>
       <c r="G142" s="8"/>
@@ -6077,7 +6069,7 @@
       <c r="K167" s="8"/>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A168" s="11"/>
+      <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="C168" s="8"/>
       <c r="D168" s="8"/>
@@ -6090,7 +6082,7 @@
       <c r="K168" s="8"/>
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A169" s="11"/>
+      <c r="A169" s="8"/>
       <c r="B169" s="8"/>
       <c r="C169" s="8"/>
       <c r="D169" s="8"/>
@@ -6103,7 +6095,7 @@
       <c r="K169" s="8"/>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A170" s="11"/>
+      <c r="A170" s="8"/>
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
       <c r="D170" s="8"/>
@@ -6480,7 +6472,9 @@
       <c r="K198" s="8"/>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A199" s="8"/>
+      <c r="A199" s="27" t="s">
+        <v>146</v>
+      </c>
       <c r="B199" s="8"/>
       <c r="C199" s="8"/>
       <c r="D199" s="8"/>
@@ -6494,135 +6488,184 @@
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="8"/>
-      <c r="B200" s="8"/>
-      <c r="C200" s="8"/>
-      <c r="D200" s="8"/>
-      <c r="E200" s="8"/>
-      <c r="F200" s="8"/>
-      <c r="G200" s="8"/>
-      <c r="H200" s="8"/>
-      <c r="I200" s="8"/>
+      <c r="B200" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C200" s="8">
+        <v>2.4647809999999999</v>
+      </c>
+      <c r="D200" s="8">
+        <v>-24.636981921705296</v>
+      </c>
+      <c r="E200" s="8">
+        <v>24.413129317131407</v>
+      </c>
+      <c r="F200" s="8">
+        <v>0.50454471874999995</v>
+      </c>
+      <c r="G200" s="8">
+        <v>-2.4926456157468602</v>
+      </c>
+      <c r="H200" s="8">
+        <v>2.820538783551894</v>
+      </c>
+      <c r="I200" s="8">
+        <f t="shared" ref="I200:I211" si="0">E200/H200</f>
+        <v>8.6554843562151067</v>
+      </c>
       <c r="J200" s="8"/>
       <c r="K200" s="8"/>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A201" s="8"/>
-      <c r="B201" s="8"/>
-      <c r="C201" s="8"/>
-      <c r="D201" s="8"/>
-      <c r="E201" s="8"/>
-      <c r="F201" s="8"/>
-      <c r="G201" s="8"/>
-      <c r="H201" s="8"/>
-      <c r="I201" s="8"/>
+      <c r="A201" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C201" s="8">
+        <v>4.086735</v>
+      </c>
+      <c r="D201" s="8">
+        <v>-23.439947666504803</v>
+      </c>
+      <c r="E201" s="8">
+        <v>40.871679420060886</v>
+      </c>
+      <c r="F201" s="8">
+        <v>1.121909375</v>
+      </c>
+      <c r="G201" s="8">
+        <v>-2.5427121504569907</v>
+      </c>
+      <c r="H201" s="8">
+        <v>6.6487742607174525</v>
+      </c>
+      <c r="I201" s="8">
+        <f t="shared" si="0"/>
+        <v>6.147250277624936</v>
+      </c>
       <c r="J201" s="8"/>
       <c r="K201" s="8"/>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A202" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="B202" s="8"/>
-      <c r="C202" s="8"/>
-      <c r="D202" s="8"/>
-      <c r="E202" s="8"/>
-      <c r="F202" s="8"/>
-      <c r="G202" s="8"/>
-      <c r="H202" s="8"/>
-      <c r="I202" s="8"/>
+      <c r="A202" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C202" s="8">
+        <v>3.7885154999999999</v>
+      </c>
+      <c r="D202" s="8">
+        <v>-22.097577142436453</v>
+      </c>
+      <c r="E202" s="8">
+        <v>37.662421709868447</v>
+      </c>
+      <c r="F202" s="8">
+        <v>1.2931708749999999</v>
+      </c>
+      <c r="G202" s="8">
+        <v>-2.8676162434251706</v>
+      </c>
+      <c r="H202" s="8">
+        <v>7.5615178062893111</v>
+      </c>
+      <c r="I202" s="8">
+        <f t="shared" si="0"/>
+        <v>4.980801827715414</v>
+      </c>
       <c r="J202" s="8"/>
       <c r="K202" s="8"/>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="8"/>
       <c r="B203" s="8" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C203" s="8">
-        <v>2.4647809999999999</v>
+        <v>1.0153720625</v>
       </c>
       <c r="D203" s="8">
-        <v>-24.636981921705296</v>
+        <v>-22.077600369598802</v>
       </c>
       <c r="E203" s="8">
-        <v>24.413129317131407</v>
+        <v>10.069834750504727</v>
       </c>
       <c r="F203" s="8">
-        <v>0.50454471874999995</v>
+        <v>0.43422881250000001</v>
       </c>
       <c r="G203" s="8">
-        <v>-2.4926456157468602</v>
+        <v>-3.2253001130414809</v>
       </c>
       <c r="H203" s="8">
-        <v>2.820538783551894</v>
+        <v>2.4406812522101879</v>
       </c>
       <c r="I203" s="8">
-        <f t="shared" ref="I203:I214" si="0">E203/H203</f>
-        <v>8.6554843562151067</v>
+        <f t="shared" si="0"/>
+        <v>4.1258295164048429</v>
       </c>
       <c r="J203" s="8"/>
       <c r="K203" s="8"/>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A204" s="11" t="s">
-        <v>149</v>
-      </c>
+      <c r="A204" s="8"/>
       <c r="B204" s="8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C204" s="8">
-        <v>4.086735</v>
+        <v>1.406757</v>
       </c>
       <c r="D204" s="8">
-        <v>-23.439947666504803</v>
+        <v>-22.849294845599655</v>
       </c>
       <c r="E204" s="8">
-        <v>40.871679420060886</v>
+        <v>14.026008338174838</v>
       </c>
       <c r="F204" s="8">
-        <v>1.121909375</v>
+        <v>0.38074456249999999</v>
       </c>
       <c r="G204" s="8">
-        <v>-2.5427121504569907</v>
+        <v>-2.1078840774540004</v>
       </c>
       <c r="H204" s="8">
-        <v>6.6487742607174525</v>
+        <v>2.1537697681782588</v>
       </c>
       <c r="I204" s="8">
         <f t="shared" si="0"/>
-        <v>6.147250277624936</v>
+        <v>6.5123062573389978</v>
       </c>
       <c r="J204" s="8"/>
       <c r="K204" s="8"/>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A205" s="11" t="s">
-        <v>151</v>
-      </c>
+      <c r="A205" s="8"/>
       <c r="B205" s="8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C205" s="8">
-        <v>3.7885154999999999</v>
+        <v>1.6791856249999999</v>
       </c>
       <c r="D205" s="8">
-        <v>-22.097577142436453</v>
+        <v>-23.586675819432717</v>
       </c>
       <c r="E205" s="8">
-        <v>37.662421709868447</v>
+        <v>16.710012880397688</v>
       </c>
       <c r="F205" s="8">
-        <v>1.2931708749999999</v>
+        <v>0.44691500000000001</v>
       </c>
       <c r="G205" s="8">
-        <v>-2.8676162434251706</v>
+        <v>-2.4747612787137325</v>
       </c>
       <c r="H205" s="8">
-        <v>7.5615178062893111</v>
+        <v>2.5130805178571953</v>
       </c>
       <c r="I205" s="8">
         <f t="shared" si="0"/>
-        <v>4.980801827715414</v>
+        <v>6.649215081515039</v>
       </c>
       <c r="J205" s="8"/>
       <c r="K205" s="8"/>
@@ -6630,29 +6673,29 @@
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="8"/>
       <c r="B206" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C206" s="8">
-        <v>1.0153720625</v>
+        <v>2.2449762500000001</v>
       </c>
       <c r="D206" s="8">
-        <v>-22.077600369598802</v>
+        <v>-21.280832426093028</v>
       </c>
       <c r="E206" s="8">
-        <v>10.069834750504727</v>
+        <v>22.274567650112381</v>
       </c>
       <c r="F206" s="8">
-        <v>0.43422881250000001</v>
+        <v>0.85107431249999999</v>
       </c>
       <c r="G206" s="8">
-        <v>-3.2253001130414809</v>
+        <v>-2.5039809809083358</v>
       </c>
       <c r="H206" s="8">
-        <v>2.4406812522101879</v>
+        <v>5.0972676622423885</v>
       </c>
       <c r="I206" s="8">
         <f t="shared" si="0"/>
-        <v>4.1258295164048429</v>
+        <v>4.3699034710516571</v>
       </c>
       <c r="J206" s="8"/>
       <c r="K206" s="8"/>
@@ -6660,29 +6703,29 @@
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="8"/>
       <c r="B207" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C207" s="8">
-        <v>1.406757</v>
+        <v>1.14325875</v>
       </c>
       <c r="D207" s="8">
-        <v>-22.849294845599655</v>
+        <v>-21.771636052368539</v>
       </c>
       <c r="E207" s="8">
-        <v>14.026008338174838</v>
+        <v>11.269680484329079</v>
       </c>
       <c r="F207" s="8">
-        <v>0.38074456249999999</v>
+        <v>0.538938625</v>
       </c>
       <c r="G207" s="8">
-        <v>-2.1078840774540004</v>
+        <v>-3.4603777000558762</v>
       </c>
       <c r="H207" s="8">
-        <v>2.1537697681782588</v>
+        <v>3.3743353176193995</v>
       </c>
       <c r="I207" s="8">
         <f t="shared" si="0"/>
-        <v>6.5123062573389978</v>
+        <v>3.339822342339072</v>
       </c>
       <c r="J207" s="8"/>
       <c r="K207" s="8"/>
@@ -6690,29 +6733,29 @@
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="8"/>
       <c r="B208" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C208" s="8">
-        <v>1.6791856249999999</v>
+        <v>13.547675</v>
       </c>
       <c r="D208" s="8">
-        <v>-23.586675819432717</v>
+        <v>-23.384482656494377</v>
       </c>
       <c r="E208" s="8">
-        <v>16.710012880397688</v>
-      </c>
-      <c r="F208" s="8">
-        <v>0.44691500000000001</v>
-      </c>
-      <c r="G208" s="8">
-        <v>-2.4747612787137325</v>
-      </c>
-      <c r="H208" s="8">
-        <v>2.5130805178571953</v>
+        <v>139.66990690416355</v>
+      </c>
+      <c r="F208" s="12">
+        <v>0.14594550000000001</v>
+      </c>
+      <c r="G208" s="12">
+        <v>0.5061024306587123</v>
+      </c>
+      <c r="H208" s="11">
+        <v>0.68921154876331958</v>
       </c>
       <c r="I208" s="8">
         <f t="shared" si="0"/>
-        <v>6.649215081515039</v>
+        <v>202.65172160097865</v>
       </c>
       <c r="J208" s="8"/>
       <c r="K208" s="8"/>
@@ -6720,29 +6763,29 @@
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="8"/>
       <c r="B209" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C209" s="8">
-        <v>2.2449762500000001</v>
+        <v>3.5904205</v>
       </c>
       <c r="D209" s="8">
-        <v>-21.280832426093028</v>
+        <v>-25.465355610572061</v>
       </c>
       <c r="E209" s="8">
-        <v>22.274567650112381</v>
+        <v>37.898644968431448</v>
       </c>
       <c r="F209" s="8">
-        <v>0.85107431249999999</v>
+        <v>0.36243106250000001</v>
       </c>
       <c r="G209" s="8">
-        <v>-2.5039809809083358</v>
+        <v>-1.4003271996130562</v>
       </c>
       <c r="H209" s="8">
-        <v>5.0972676622423885</v>
+        <v>1.9955317705006792</v>
       </c>
       <c r="I209" s="8">
         <f t="shared" si="0"/>
-        <v>4.3699034710516571</v>
+        <v>18.991752238012563</v>
       </c>
       <c r="J209" s="8"/>
       <c r="K209" s="8"/>
@@ -6750,29 +6793,29 @@
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="8"/>
       <c r="B210" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C210" s="8">
-        <v>1.14325875</v>
+        <v>4.0976105</v>
       </c>
       <c r="D210" s="8">
-        <v>-21.771636052368539</v>
+        <v>-25.814627939437877</v>
       </c>
       <c r="E210" s="8">
-        <v>11.269680484329079</v>
+        <v>41.378601491432562</v>
       </c>
       <c r="F210" s="8">
-        <v>0.538938625</v>
+        <v>0.30305431249999998</v>
       </c>
       <c r="G210" s="8">
-        <v>-3.4603777000558762</v>
+        <v>-1.8011910864977838</v>
       </c>
       <c r="H210" s="8">
-        <v>3.3743353176193995</v>
+        <v>1.6869969879309739</v>
       </c>
       <c r="I210" s="8">
         <f t="shared" si="0"/>
-        <v>3.339822342339072</v>
+        <v>24.527964061264601</v>
       </c>
       <c r="J210" s="8"/>
       <c r="K210" s="8"/>
@@ -6780,323 +6823,298 @@
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="8"/>
       <c r="B211" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C211" s="8">
-        <v>13.547675</v>
+        <v>5.5374129999999999</v>
       </c>
       <c r="D211" s="8">
-        <v>-23.384482656494377</v>
+        <v>-25.577633398068887</v>
       </c>
       <c r="E211" s="8">
-        <v>139.66990690416355</v>
-      </c>
-      <c r="F211" s="12">
-        <v>0.14594550000000001</v>
-      </c>
-      <c r="G211" s="12">
-        <v>0.5061024306587123</v>
-      </c>
-      <c r="H211" s="11">
-        <v>0.68921154876331958</v>
+        <v>54.483894864536282</v>
+      </c>
+      <c r="F211" s="8">
+        <v>0.30616650000000001</v>
+      </c>
+      <c r="G211" s="8">
+        <v>-0.75974281139207223</v>
+      </c>
+      <c r="H211" s="8">
+        <v>1.6807086879933379</v>
       </c>
       <c r="I211" s="8">
         <f t="shared" si="0"/>
-        <v>202.65172160097865</v>
+        <v>32.417214984225893</v>
       </c>
       <c r="J211" s="8"/>
       <c r="K211" s="8"/>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="8"/>
-      <c r="B212" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C212" s="8">
-        <v>3.5904205</v>
-      </c>
-      <c r="D212" s="8">
-        <v>-25.465355610572061</v>
-      </c>
-      <c r="E212" s="8">
-        <v>37.898644968431448</v>
-      </c>
-      <c r="F212" s="8">
-        <v>0.36243106250000001</v>
-      </c>
-      <c r="G212" s="8">
-        <v>-1.4003271996130562</v>
-      </c>
-      <c r="H212" s="8">
-        <v>1.9955317705006792</v>
-      </c>
-      <c r="I212" s="8">
-        <f t="shared" si="0"/>
-        <v>18.991752238012563</v>
-      </c>
+      <c r="B212" s="8"/>
+      <c r="C212" s="8"/>
+      <c r="D212" s="8"/>
+      <c r="E212" s="8"/>
+      <c r="F212" s="8"/>
+      <c r="G212" s="8"/>
+      <c r="H212" s="8"/>
+      <c r="I212" s="8"/>
       <c r="J212" s="8"/>
       <c r="K212" s="8"/>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="8"/>
-      <c r="B213" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C213" s="8">
-        <v>4.0976105</v>
-      </c>
-      <c r="D213" s="8">
-        <v>-25.814627939437877</v>
-      </c>
-      <c r="E213" s="8">
-        <v>41.378601491432562</v>
-      </c>
-      <c r="F213" s="8">
-        <v>0.30305431249999998</v>
-      </c>
-      <c r="G213" s="8">
-        <v>-1.8011910864977838</v>
-      </c>
-      <c r="H213" s="8">
-        <v>1.6869969879309739</v>
-      </c>
-      <c r="I213" s="8">
-        <f t="shared" si="0"/>
-        <v>24.527964061264601</v>
-      </c>
+      <c r="B213" s="8"/>
+      <c r="C213" s="8"/>
+      <c r="D213" s="8"/>
+      <c r="E213" s="8"/>
+      <c r="F213" s="8"/>
+      <c r="G213" s="8"/>
+      <c r="H213" s="8"/>
+      <c r="I213" s="8"/>
       <c r="J213" s="8"/>
       <c r="K213" s="8"/>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="8"/>
-      <c r="B214" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C214" s="8">
-        <v>5.5374129999999999</v>
-      </c>
-      <c r="D214" s="8">
-        <v>-25.577633398068887</v>
-      </c>
-      <c r="E214" s="8">
-        <v>54.483894864536282</v>
-      </c>
-      <c r="F214" s="8">
-        <v>0.30616650000000001</v>
-      </c>
-      <c r="G214" s="8">
-        <v>-0.75974281139207223</v>
-      </c>
-      <c r="H214" s="8">
-        <v>1.6807086879933379</v>
-      </c>
-      <c r="I214" s="8">
-        <f t="shared" si="0"/>
-        <v>32.417214984225893</v>
-      </c>
+      <c r="B214" s="8"/>
+      <c r="C214" s="8"/>
+      <c r="D214" s="8"/>
+      <c r="E214" s="8"/>
+      <c r="F214" s="8"/>
+      <c r="G214" s="8"/>
+      <c r="H214" s="8"/>
+      <c r="I214" s="8"/>
       <c r="J214" s="8"/>
       <c r="K214" s="8"/>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A215" s="8"/>
-      <c r="B215" s="8"/>
-      <c r="C215" s="8"/>
-      <c r="D215" s="8"/>
-      <c r="E215" s="8"/>
-      <c r="F215" s="8"/>
-      <c r="G215" s="8"/>
-      <c r="H215" s="8"/>
+      <c r="A215" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B215" s="8">
+        <v>2.2533655000000001</v>
+      </c>
+      <c r="C215" s="8">
+        <v>-21.805154109235776</v>
+      </c>
+      <c r="D215" s="8">
+        <v>20.82862554090778</v>
+      </c>
+      <c r="E215" s="8">
+        <v>1.084314875</v>
+      </c>
+      <c r="F215" s="8">
+        <v>6.1404625372728852</v>
+      </c>
+      <c r="G215" s="8">
+        <v>5.7828027254556416</v>
+      </c>
+      <c r="H215" s="8">
+        <f t="shared" ref="H215:H225" si="1">D215/G215</f>
+        <v>3.6018219070868684</v>
+      </c>
       <c r="I215" s="8"/>
       <c r="J215" s="8"/>
       <c r="K215" s="8"/>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A216" s="8"/>
-      <c r="B216" s="8"/>
-      <c r="C216" s="8"/>
-      <c r="D216" s="8"/>
-      <c r="E216" s="8"/>
-      <c r="F216" s="8"/>
-      <c r="G216" s="8"/>
-      <c r="H216" s="8"/>
+      <c r="A216" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B216" s="8">
+        <v>3.13893025</v>
+      </c>
+      <c r="C216" s="8">
+        <v>-21.842773889704841</v>
+      </c>
+      <c r="D216" s="8">
+        <v>29.069591745721933</v>
+      </c>
+      <c r="E216" s="8">
+        <v>1.4801599999999999</v>
+      </c>
+      <c r="F216" s="8">
+        <v>6.3572785122755304</v>
+      </c>
+      <c r="G216" s="8">
+        <v>7.7239970287710316</v>
+      </c>
+      <c r="H216" s="8">
+        <f t="shared" si="1"/>
+        <v>3.7635425851979138</v>
+      </c>
       <c r="I216" s="8"/>
       <c r="J216" s="8"/>
       <c r="K216" s="8"/>
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A217" s="8"/>
-      <c r="B217" s="8"/>
-      <c r="C217" s="8"/>
-      <c r="D217" s="8"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="G217" s="8"/>
-      <c r="H217" s="8"/>
+      <c r="A217" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B217" s="8">
+        <v>2.5602024999999999</v>
+      </c>
+      <c r="C217" s="8">
+        <v>-22.230924646242656</v>
+      </c>
+      <c r="D217" s="8">
+        <v>24.578582962075636</v>
+      </c>
+      <c r="E217" s="8">
+        <v>1.211476875</v>
+      </c>
+      <c r="F217" s="8">
+        <v>5.7280320488410919</v>
+      </c>
+      <c r="G217" s="8">
+        <v>6.3840084641621093</v>
+      </c>
+      <c r="H217" s="8">
+        <f t="shared" si="1"/>
+        <v>3.8500235549580424</v>
+      </c>
       <c r="I217" s="8"/>
       <c r="J217" s="8"/>
       <c r="K217" s="8"/>
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A218" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B218" s="8">
-        <v>2.2533655000000001</v>
-      </c>
-      <c r="C218" s="8">
-        <v>-21.805154109235776</v>
-      </c>
-      <c r="D218" s="8">
-        <v>20.82862554090778</v>
-      </c>
-      <c r="E218" s="8">
-        <v>1.084314875</v>
-      </c>
-      <c r="F218" s="8">
-        <v>6.1404625372728852</v>
-      </c>
-      <c r="G218" s="8">
-        <v>5.7828027254556416</v>
-      </c>
-      <c r="H218" s="8">
-        <f t="shared" ref="H218:H228" si="1">D218/G218</f>
-        <v>3.6018219070868684</v>
+      <c r="A218" s="8"/>
+      <c r="B218" s="8"/>
+      <c r="C218" s="27">
+        <f>AVERAGE(C215:C217)</f>
+        <v>-21.959617548394423</v>
+      </c>
+      <c r="D218" s="27"/>
+      <c r="E218" s="27"/>
+      <c r="F218" s="27">
+        <f>AVERAGE(F215:F217)</f>
+        <v>6.0752576994631697</v>
+      </c>
+      <c r="G218" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="H218" s="27">
+        <f>COUNT(H215:H217)</f>
+        <v>3</v>
       </c>
       <c r="I218" s="8"/>
       <c r="J218" s="8"/>
       <c r="K218" s="8"/>
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A219" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B219" s="8">
-        <v>3.13893025</v>
-      </c>
-      <c r="C219" s="8">
-        <v>-21.842773889704841</v>
-      </c>
-      <c r="D219" s="8">
-        <v>29.069591745721933</v>
-      </c>
-      <c r="E219" s="8">
-        <v>1.4801599999999999</v>
-      </c>
-      <c r="F219" s="8">
-        <v>6.3572785122755304</v>
-      </c>
-      <c r="G219" s="8">
-        <v>7.7239970287710316</v>
-      </c>
-      <c r="H219" s="8">
-        <f t="shared" si="1"/>
-        <v>3.7635425851979138</v>
+      <c r="A219" s="8"/>
+      <c r="B219" s="8"/>
+      <c r="C219" s="27">
+        <f>_xlfn.STDEV.S(C215:C217)</f>
+        <v>0.2357105597502106</v>
+      </c>
+      <c r="D219" s="27"/>
+      <c r="E219" s="27"/>
+      <c r="F219" s="27">
+        <f>_xlfn.STDEV.S(F215:F217)</f>
+        <v>0.31965063912266872</v>
+      </c>
+      <c r="G219" s="27"/>
+      <c r="H219" s="27">
+        <f>_xlfn.STDEV.S(H215:H217)</f>
+        <v>0.12598716460107806</v>
       </c>
       <c r="I219" s="8"/>
       <c r="J219" s="8"/>
       <c r="K219" s="8"/>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A220" s="8" t="s">
+      <c r="A220" t="s">
         <v>56</v>
       </c>
-      <c r="B220" s="8">
-        <v>2.5602024999999999</v>
-      </c>
-      <c r="C220" s="8">
-        <v>-22.230924646242656</v>
-      </c>
-      <c r="D220" s="8">
-        <v>24.578582962075636</v>
-      </c>
-      <c r="E220" s="8">
-        <v>1.211476875</v>
-      </c>
-      <c r="F220" s="8">
-        <v>5.7280320488410919</v>
-      </c>
-      <c r="G220" s="8">
-        <v>6.3840084641621093</v>
-      </c>
-      <c r="H220" s="8">
-        <f t="shared" si="1"/>
-        <v>3.8500235549580424</v>
-      </c>
-      <c r="I220" s="8"/>
-      <c r="J220" s="8"/>
-      <c r="K220" s="8"/>
-    </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A221" s="8"/>
-      <c r="B221" s="8"/>
-      <c r="C221" s="27">
-        <f>AVERAGE(C218:C220)</f>
-        <v>-21.959617548394423</v>
-      </c>
-      <c r="D221" s="27"/>
-      <c r="E221" s="27"/>
-      <c r="F221" s="27">
-        <f>AVERAGE(F218:F220)</f>
-        <v>6.0752576994631697</v>
-      </c>
-      <c r="G221" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="H221" s="27">
-        <f>COUNT(H218:H220)</f>
-        <v>3</v>
-      </c>
-      <c r="I221" s="8"/>
-      <c r="J221" s="8"/>
-      <c r="K221" s="8"/>
-    </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A222" s="8"/>
-      <c r="B222" s="8"/>
-      <c r="C222" s="27">
-        <f>_xlfn.STDEV.S(C218:C220)</f>
-        <v>0.2357105597502106</v>
-      </c>
-      <c r="D222" s="27"/>
-      <c r="E222" s="27"/>
-      <c r="F222" s="27">
-        <f>_xlfn.STDEV.S(F218:F220)</f>
-        <v>0.31965063912266872</v>
-      </c>
-      <c r="G222" s="27"/>
-      <c r="H222" s="27">
-        <f>_xlfn.STDEV.S(H218:H220)</f>
-        <v>0.12598716460107806</v>
-      </c>
-      <c r="I222" s="8"/>
-      <c r="J222" s="8"/>
-      <c r="K222" s="8"/>
-    </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>57</v>
-      </c>
-      <c r="B223">
+      <c r="B220">
         <v>1.2257828749999999</v>
       </c>
-      <c r="C223" s="4">
+      <c r="C220" s="4">
         <v>-21.758250523484364</v>
       </c>
-      <c r="D223" s="1">
+      <c r="D220" s="1">
         <v>11.92509375852884</v>
       </c>
-      <c r="E223">
+      <c r="E220">
         <v>0.62290599999999996</v>
       </c>
-      <c r="F223" s="2">
+      <c r="F220" s="2">
         <v>4.5472199764748922</v>
       </c>
-      <c r="G223" s="3">
+      <c r="G220" s="3">
         <v>3.4676954043990995</v>
       </c>
-      <c r="H223" s="4">
+      <c r="H220" s="4">
         <f t="shared" si="1"/>
         <v>3.4389103908609537</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>57</v>
+      </c>
+      <c r="B221">
+        <v>0.59160000000000001</v>
+      </c>
+      <c r="C221" s="4">
+        <v>-21.637299550087707</v>
+      </c>
+      <c r="D221" s="1">
+        <v>5.8826242384347562</v>
+      </c>
+      <c r="E221">
+        <v>0.31186671874999999</v>
+      </c>
+      <c r="F221" s="2">
+        <v>4.0773963636830945</v>
+      </c>
+      <c r="G221" s="3">
+        <v>1.8942994443017684</v>
+      </c>
+      <c r="H221" s="4">
+        <f t="shared" si="1"/>
+        <v>3.1054352341865723</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C222" s="13">
+        <f>AVERAGE(C220:C221)</f>
+        <v>-21.697775036786034</v>
+      </c>
+      <c r="D222" s="14"/>
+      <c r="E222" s="9"/>
+      <c r="F222" s="15">
+        <f>AVERAGE(F220:F221)</f>
+        <v>4.3123081700789934</v>
+      </c>
+      <c r="G222" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H222" s="13">
+        <f>AVERAGE(H220:H221)</f>
+        <v>3.2721728125237632</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C223" s="13">
+        <f>_xlfn.STDEV.S(C220:C221)</f>
+        <v>8.552525347988936E-2</v>
+      </c>
+      <c r="D223" s="14"/>
+      <c r="E223" s="9"/>
+      <c r="F223" s="15">
+        <f>_xlfn.STDEV.S(F220:F221)</f>
+        <v>0.33221546256664286</v>
+      </c>
+      <c r="G223" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="H223" s="13">
+        <f>_xlfn.STDEV.S(H220:H221)</f>
+        <v>0.2358025446417015</v>
       </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
@@ -7104,158 +7122,93 @@
         <v>58</v>
       </c>
       <c r="B224">
-        <v>0.59160000000000001</v>
+        <v>4.1791697499999998</v>
       </c>
       <c r="C224" s="4">
-        <v>-21.637299550087707</v>
+        <v>-24.119495252647759</v>
       </c>
       <c r="D224" s="1">
-        <v>5.8826242384347562</v>
+        <v>40.028383812374337</v>
       </c>
       <c r="E224">
-        <v>0.31186671874999999</v>
+        <v>1.298635625</v>
       </c>
       <c r="F224" s="2">
-        <v>4.0773963636830945</v>
+        <v>5.1051442348992726</v>
       </c>
       <c r="G224" s="3">
-        <v>1.8942994443017684</v>
+        <v>6.8031716098956672</v>
       </c>
       <c r="H224" s="4">
         <f t="shared" si="1"/>
-        <v>3.1054352341865723</v>
+        <v>5.8837827571702555</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C225" s="13">
-        <f>AVERAGE(C223:C224)</f>
-        <v>-21.697775036786034</v>
-      </c>
-      <c r="D225" s="14"/>
-      <c r="E225" s="9"/>
-      <c r="F225" s="15">
-        <f>AVERAGE(F223:F224)</f>
-        <v>4.3123081700789934</v>
-      </c>
-      <c r="G225" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H225" s="13">
-        <f>AVERAGE(H223:H224)</f>
-        <v>3.2721728125237632</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C226" s="13">
-        <f>_xlfn.STDEV.S(C223:C224)</f>
-        <v>8.552525347988936E-2</v>
-      </c>
-      <c r="D226" s="14"/>
-      <c r="E226" s="9"/>
-      <c r="F226" s="15">
-        <f>_xlfn.STDEV.S(F223:F224)</f>
-        <v>0.33221546256664286</v>
-      </c>
-      <c r="G226" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="H226" s="13">
-        <f>_xlfn.STDEV.S(H223:H224)</f>
-        <v>0.2358025446417015</v>
-      </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A227" t="s">
+      <c r="A225" t="s">
         <v>59</v>
       </c>
-      <c r="B227">
-        <v>4.1791697499999998</v>
-      </c>
-      <c r="C227" s="4">
-        <v>-24.119495252647759</v>
-      </c>
-      <c r="D227" s="1">
-        <v>40.028383812374337</v>
-      </c>
-      <c r="E227">
-        <v>1.298635625</v>
-      </c>
-      <c r="F227" s="2">
-        <v>5.1051442348992726</v>
-      </c>
-      <c r="G227" s="3">
-        <v>6.8031716098956672</v>
-      </c>
-      <c r="H227" s="4">
-        <f t="shared" si="1"/>
-        <v>5.8837827571702555</v>
-      </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>60</v>
-      </c>
-      <c r="B228">
+      <c r="B225">
         <v>3.9981452499999999</v>
       </c>
-      <c r="C228" s="4">
+      <c r="C225" s="4">
         <v>-24.734714842780214</v>
       </c>
-      <c r="D228" s="1">
+      <c r="D225" s="1">
         <v>38.903565205554017</v>
       </c>
-      <c r="E228">
+      <c r="E225">
         <v>1.0060871874999999</v>
       </c>
-      <c r="F228" s="2">
+      <c r="F225" s="2">
         <v>5.1378309970462333</v>
       </c>
-      <c r="G228" s="3">
+      <c r="G225" s="3">
         <v>5.3554382407699039</v>
       </c>
-      <c r="H228" s="4">
+      <c r="H225" s="4">
         <f t="shared" si="1"/>
         <v>7.2643103059967684</v>
       </c>
-      <c r="I228" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C229" s="9">
-        <f>AVERAGE(C227:C228)</f>
+      <c r="I225" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C226" s="9">
+        <f>AVERAGE(C224:C225)</f>
         <v>-24.427105047713987</v>
       </c>
-      <c r="D229" s="9"/>
-      <c r="E229" s="14"/>
-      <c r="F229" s="9">
-        <f>AVERAGE(F227:F228)</f>
+      <c r="D226" s="9"/>
+      <c r="E226" s="14"/>
+      <c r="F226" s="9">
+        <f>AVERAGE(F224:F225)</f>
         <v>5.1214876159727529</v>
       </c>
-      <c r="G229" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H229" s="16">
-        <f>AVERAGE(H227:H228)</f>
+      <c r="G226" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H226" s="16">
+        <f>AVERAGE(H224:H225)</f>
         <v>6.5740465315835124</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C230" s="9">
-        <f>_xlfn.STDEV.S(C227:C228)</f>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C227" s="9">
+        <f>_xlfn.STDEV.S(C224:C225)</f>
         <v>0.43502594410146705</v>
       </c>
-      <c r="D230" s="9"/>
-      <c r="E230" s="14"/>
-      <c r="F230" s="9">
-        <f>_xlfn.STDEV.S(F227:F228)</f>
+      <c r="D227" s="9"/>
+      <c r="E227" s="14"/>
+      <c r="F227" s="9">
+        <f>_xlfn.STDEV.S(F224:F225)</f>
         <v>2.3113031169147626E-2</v>
       </c>
-      <c r="G230" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="H230" s="16">
-        <f>_xlfn.STDEV.S(H227:H228)</f>
+      <c r="G227" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H227" s="16">
+        <f>_xlfn.STDEV.S(H224:H225)</f>
         <v>0.97618039139006929</v>
       </c>
     </row>

</xml_diff>